<commit_message>
Einführen eines neuen Projekt Reports : Übersicht Vergleich mit letztem stand, Beauftragung ; calculateRoundedKPI Funktion eingeführt, damit immer die gleichen Werte zu Ergebnis, Personalkosten, etc herauskommen; listdifferences Methode in clsprojkt angepasst
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/bin/Debug/requirements/Project Board Customization.xlsx
+++ b/Projectboard/Projectboard/bin/Debug/requirements/Project Board Customization.xlsx
@@ -605,7 +605,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -710,12 +710,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -769,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -799,9 +793,8 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -809,12 +802,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1167,7 +1160,7 @@
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1173,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1188,17 +1181,17 @@
       <c r="A3" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="40" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1213,12 +1206,12 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1228,7 +1221,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1238,7 +1231,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1256,417 +1249,417 @@
       <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="30">
         <f>Start_Kalender</f>
         <v>41153</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="30">
         <v>41183</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="30">
         <v>41214</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="30">
         <v>41244</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="30">
         <v>41275</v>
       </c>
-      <c r="K17" s="31">
+      <c r="K17" s="30">
         <v>41306</v>
       </c>
-      <c r="L17" s="31">
+      <c r="L17" s="30">
         <v>41334</v>
       </c>
-      <c r="M17" s="31">
+      <c r="M17" s="30">
         <v>41365</v>
       </c>
-      <c r="N17" s="31">
+      <c r="N17" s="30">
         <v>41395</v>
       </c>
-      <c r="O17" s="31">
+      <c r="O17" s="30">
         <v>41426</v>
       </c>
-      <c r="P17" s="31">
+      <c r="P17" s="30">
         <v>41456</v>
       </c>
-      <c r="Q17" s="31">
+      <c r="Q17" s="30">
         <v>41487</v>
       </c>
-      <c r="R17" s="31">
+      <c r="R17" s="30">
         <v>41518</v>
       </c>
-      <c r="S17" s="31">
+      <c r="S17" s="30">
         <v>41548</v>
       </c>
-      <c r="T17" s="31">
+      <c r="T17" s="30">
         <v>41579</v>
       </c>
-      <c r="U17" s="31">
+      <c r="U17" s="30">
         <v>41609</v>
       </c>
-      <c r="V17" s="31">
+      <c r="V17" s="30">
         <v>41640</v>
       </c>
-      <c r="W17" s="31">
+      <c r="W17" s="30">
         <v>41671</v>
       </c>
-      <c r="X17" s="31">
+      <c r="X17" s="30">
         <v>41699</v>
       </c>
-      <c r="Y17" s="31">
+      <c r="Y17" s="30">
         <v>41730</v>
       </c>
-      <c r="Z17" s="31">
+      <c r="Z17" s="30">
         <v>41760</v>
       </c>
-      <c r="AA17" s="31">
+      <c r="AA17" s="30">
         <v>41791</v>
       </c>
-      <c r="AB17" s="31">
+      <c r="AB17" s="30">
         <v>41821</v>
       </c>
-      <c r="AC17" s="31">
+      <c r="AC17" s="30">
         <v>41852</v>
       </c>
-      <c r="AD17" s="31">
+      <c r="AD17" s="30">
         <v>41883</v>
       </c>
-      <c r="AE17" s="31">
+      <c r="AE17" s="30">
         <v>41913</v>
       </c>
-      <c r="AF17" s="31">
+      <c r="AF17" s="30">
         <v>41944</v>
       </c>
-      <c r="AG17" s="31">
+      <c r="AG17" s="30">
         <v>41974</v>
       </c>
-      <c r="AH17" s="31">
+      <c r="AH17" s="30">
         <v>42005</v>
       </c>
-      <c r="AI17" s="31">
+      <c r="AI17" s="30">
         <v>42036</v>
       </c>
-      <c r="AJ17" s="31">
+      <c r="AJ17" s="30">
         <v>42064</v>
       </c>
-      <c r="AK17" s="31">
+      <c r="AK17" s="30">
         <v>42095</v>
       </c>
-      <c r="AL17" s="31">
+      <c r="AL17" s="30">
         <v>42125</v>
       </c>
-      <c r="AM17" s="31">
+      <c r="AM17" s="30">
         <v>42156</v>
       </c>
-      <c r="AN17" s="31">
+      <c r="AN17" s="30">
         <v>42186</v>
       </c>
-      <c r="AO17" s="31">
+      <c r="AO17" s="30">
         <v>42217</v>
       </c>
-      <c r="AP17" s="31">
+      <c r="AP17" s="30">
         <v>42248</v>
       </c>
-      <c r="AQ17" s="31">
+      <c r="AQ17" s="30">
         <v>42278</v>
       </c>
-      <c r="AR17" s="31">
+      <c r="AR17" s="30">
         <v>42309</v>
       </c>
-      <c r="AS17" s="31">
+      <c r="AS17" s="30">
         <v>42339</v>
       </c>
-      <c r="AT17" s="31">
+      <c r="AT17" s="30">
         <v>42370</v>
       </c>
-      <c r="AU17" s="31">
+      <c r="AU17" s="30">
         <v>42401</v>
       </c>
-      <c r="AV17" s="31">
+      <c r="AV17" s="30">
         <v>42430</v>
       </c>
-      <c r="AW17" s="31">
+      <c r="AW17" s="30">
         <v>42461</v>
       </c>
-      <c r="AX17" s="31">
+      <c r="AX17" s="30">
         <v>42491</v>
       </c>
-      <c r="AY17" s="31">
+      <c r="AY17" s="30">
         <v>42522</v>
       </c>
-      <c r="AZ17" s="31">
+      <c r="AZ17" s="30">
         <v>42552</v>
       </c>
-      <c r="BA17" s="31">
+      <c r="BA17" s="30">
         <v>42583</v>
       </c>
-      <c r="BB17" s="31">
+      <c r="BB17" s="30">
         <v>42614</v>
       </c>
-      <c r="BC17" s="31">
+      <c r="BC17" s="30">
         <v>42644</v>
       </c>
-      <c r="BD17" s="31">
+      <c r="BD17" s="30">
         <v>42675</v>
       </c>
-      <c r="BE17" s="31">
+      <c r="BE17" s="30">
         <v>42705</v>
       </c>
-      <c r="BF17" s="31">
+      <c r="BF17" s="30">
         <v>42736</v>
       </c>
-      <c r="BG17" s="31">
+      <c r="BG17" s="30">
         <v>42767</v>
       </c>
-      <c r="BH17" s="31">
+      <c r="BH17" s="30">
         <v>42795</v>
       </c>
-      <c r="BI17" s="31">
+      <c r="BI17" s="30">
         <v>42826</v>
       </c>
-      <c r="BJ17" s="31">
+      <c r="BJ17" s="30">
         <v>42856</v>
       </c>
-      <c r="BK17" s="31">
+      <c r="BK17" s="30">
         <v>42887</v>
       </c>
-      <c r="BL17" s="31">
+      <c r="BL17" s="30">
         <v>42917</v>
       </c>
-      <c r="BM17" s="31">
+      <c r="BM17" s="30">
         <v>42948</v>
       </c>
-      <c r="BN17" s="31">
+      <c r="BN17" s="30">
         <v>42979</v>
       </c>
-      <c r="BO17" s="31">
+      <c r="BO17" s="30">
         <v>43009</v>
       </c>
-      <c r="BP17" s="31">
+      <c r="BP17" s="30">
         <v>43040</v>
       </c>
-      <c r="BQ17" s="31">
+      <c r="BQ17" s="30">
         <v>43070</v>
       </c>
-      <c r="BR17" s="31">
+      <c r="BR17" s="30">
         <v>43101</v>
       </c>
-      <c r="BS17" s="31">
+      <c r="BS17" s="30">
         <v>43132</v>
       </c>
-      <c r="BT17" s="31">
+      <c r="BT17" s="30">
         <v>43160</v>
       </c>
-      <c r="BU17" s="31">
+      <c r="BU17" s="30">
         <v>43191</v>
       </c>
-      <c r="BV17" s="31">
+      <c r="BV17" s="30">
         <v>43221</v>
       </c>
-      <c r="BW17" s="31">
+      <c r="BW17" s="30">
         <v>43252</v>
       </c>
-      <c r="BX17" s="31">
+      <c r="BX17" s="30">
         <v>43282</v>
       </c>
-      <c r="BY17" s="31">
+      <c r="BY17" s="30">
         <v>43313</v>
       </c>
-      <c r="BZ17" s="31">
+      <c r="BZ17" s="30">
         <v>43344</v>
       </c>
-      <c r="CA17" s="31">
+      <c r="CA17" s="30">
         <v>43374</v>
       </c>
-      <c r="CB17" s="31">
+      <c r="CB17" s="30">
         <v>43405</v>
       </c>
-      <c r="CC17" s="31">
+      <c r="CC17" s="30">
         <v>43435</v>
       </c>
-      <c r="CD17" s="31">
+      <c r="CD17" s="30">
         <v>43466</v>
       </c>
-      <c r="CE17" s="31">
+      <c r="CE17" s="30">
         <v>43497</v>
       </c>
-      <c r="CF17" s="31">
+      <c r="CF17" s="30">
         <v>43525</v>
       </c>
-      <c r="CG17" s="31">
+      <c r="CG17" s="30">
         <v>43556</v>
       </c>
-      <c r="CH17" s="31">
+      <c r="CH17" s="30">
         <v>43586</v>
       </c>
-      <c r="CI17" s="31">
+      <c r="CI17" s="30">
         <v>43617</v>
       </c>
-      <c r="CJ17" s="31">
+      <c r="CJ17" s="30">
         <v>43647</v>
       </c>
-      <c r="CK17" s="31">
+      <c r="CK17" s="30">
         <v>43678</v>
       </c>
-      <c r="CL17" s="31">
+      <c r="CL17" s="30">
         <v>43709</v>
       </c>
-      <c r="CM17" s="31">
+      <c r="CM17" s="30">
         <v>43739</v>
       </c>
-      <c r="CN17" s="31">
+      <c r="CN17" s="30">
         <v>43770</v>
       </c>
-      <c r="CO17" s="31">
+      <c r="CO17" s="30">
         <v>43800</v>
       </c>
-      <c r="CP17" s="31">
+      <c r="CP17" s="30">
         <v>43831</v>
       </c>
-      <c r="CQ17" s="31">
+      <c r="CQ17" s="30">
         <v>43862</v>
       </c>
-      <c r="CR17" s="31">
+      <c r="CR17" s="30">
         <v>43891</v>
       </c>
-      <c r="CS17" s="31">
+      <c r="CS17" s="30">
         <v>43922</v>
       </c>
-      <c r="CT17" s="31">
+      <c r="CT17" s="30">
         <v>43952</v>
       </c>
-      <c r="CU17" s="31">
+      <c r="CU17" s="30">
         <v>43983</v>
       </c>
-      <c r="CV17" s="31">
+      <c r="CV17" s="30">
         <v>44013</v>
       </c>
-      <c r="CW17" s="31">
+      <c r="CW17" s="30">
         <v>44044</v>
       </c>
-      <c r="CX17" s="31">
+      <c r="CX17" s="30">
         <v>44075</v>
       </c>
-      <c r="CY17" s="31">
+      <c r="CY17" s="30">
         <v>44105</v>
       </c>
-      <c r="CZ17" s="31">
+      <c r="CZ17" s="30">
         <v>44136</v>
       </c>
-      <c r="DA17" s="31">
+      <c r="DA17" s="30">
         <v>44166</v>
       </c>
-      <c r="DB17" s="31">
+      <c r="DB17" s="30">
         <v>44197</v>
       </c>
-      <c r="DC17" s="31">
+      <c r="DC17" s="30">
         <v>44228</v>
       </c>
-      <c r="DD17" s="31">
+      <c r="DD17" s="30">
         <v>44256</v>
       </c>
-      <c r="DE17" s="31">
+      <c r="DE17" s="30">
         <v>44287</v>
       </c>
-      <c r="DF17" s="31">
+      <c r="DF17" s="30">
         <v>44317</v>
       </c>
-      <c r="DG17" s="31">
+      <c r="DG17" s="30">
         <v>44348</v>
       </c>
-      <c r="DH17" s="31">
+      <c r="DH17" s="30">
         <v>44378</v>
       </c>
-      <c r="DI17" s="31">
+      <c r="DI17" s="30">
         <v>44409</v>
       </c>
-      <c r="DJ17" s="31">
+      <c r="DJ17" s="30">
         <v>44440</v>
       </c>
-      <c r="DK17" s="31">
+      <c r="DK17" s="30">
         <v>44470</v>
       </c>
-      <c r="DL17" s="31">
+      <c r="DL17" s="30">
         <v>44501</v>
       </c>
-      <c r="DM17" s="31">
+      <c r="DM17" s="30">
         <v>44531</v>
       </c>
-      <c r="DN17" s="31">
+      <c r="DN17" s="30">
         <v>44562</v>
       </c>
-      <c r="DO17" s="31">
+      <c r="DO17" s="30">
         <v>44593</v>
       </c>
-      <c r="DP17" s="31">
+      <c r="DP17" s="30">
         <v>44621</v>
       </c>
-      <c r="DQ17" s="31">
+      <c r="DQ17" s="30">
         <v>44652</v>
       </c>
-      <c r="DR17" s="31">
+      <c r="DR17" s="30">
         <v>44682</v>
       </c>
-      <c r="DS17" s="31">
+      <c r="DS17" s="30">
         <v>44713</v>
       </c>
-      <c r="DT17" s="31">
+      <c r="DT17" s="30">
         <v>44743</v>
       </c>
-      <c r="DU17" s="31">
+      <c r="DU17" s="30">
         <v>44774</v>
       </c>
-      <c r="DV17" s="31">
+      <c r="DV17" s="30">
         <v>44805</v>
       </c>
-      <c r="DW17" s="31">
+      <c r="DW17" s="30">
         <v>44835</v>
       </c>
-      <c r="DX17" s="31">
+      <c r="DX17" s="30">
         <v>44866</v>
       </c>
-      <c r="DY17" s="31">
+      <c r="DY17" s="30">
         <v>44896</v>
       </c>
-      <c r="DZ17" s="31">
+      <c r="DZ17" s="30">
         <v>44927</v>
       </c>
-      <c r="EA17" s="31">
+      <c r="EA17" s="30">
         <v>44958</v>
       </c>
-      <c r="EB17" s="31">
+      <c r="EB17" s="30">
         <v>44986</v>
       </c>
-      <c r="EC17" s="31">
+      <c r="EC17" s="30">
         <v>45017</v>
       </c>
-      <c r="ED17" s="31">
+      <c r="ED17" s="30">
         <v>45047</v>
       </c>
-      <c r="EE17" s="31">
+      <c r="EE17" s="30">
         <v>45078</v>
       </c>
-      <c r="EF17" s="31">
+      <c r="EF17" s="30">
         <v>45108</v>
       </c>
-      <c r="EG17" s="31">
+      <c r="EG17" s="30">
         <v>45139</v>
       </c>
-      <c r="EH17" s="31"/>
-      <c r="EI17" s="31"/>
+      <c r="EH17" s="30"/>
+      <c r="EI17" s="30"/>
     </row>
     <row r="18" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="7">
@@ -2727,7 +2720,7 @@
       </c>
     </row>
     <row r="20" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="28" t="s">
         <v>118</v>
       </c>
       <c r="C20" s="7">
@@ -3249,7 +3242,7 @@
       </c>
     </row>
     <row r="21" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>127</v>
       </c>
       <c r="C21" s="7">
@@ -3771,7 +3764,7 @@
       </c>
     </row>
     <row r="22" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>119</v>
       </c>
       <c r="C22" s="7">
@@ -4838,7 +4831,7 @@
       </c>
     </row>
     <row r="29" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="42" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4846,7 +4839,7 @@
       <c r="A30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="37"/>
+      <c r="B30" s="36"/>
     </row>
     <row r="31" spans="1:139" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
@@ -4980,19 +4973,19 @@
       <c r="A54" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="35"/>
+      <c r="B54" s="34"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>97</v>
       </c>
-      <c r="B55" s="36"/>
+      <c r="B55" s="35"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>98</v>
       </c>
-      <c r="B56" s="37"/>
+      <c r="B56" s="36"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -5004,7 +4997,7 @@
       <c r="A58" t="s">
         <v>101</v>
       </c>
-      <c r="B58" s="27"/>
+      <c r="B58" s="36"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -5112,7 +5105,7 @@
       <c r="A68" t="s">
         <v>109</v>
       </c>
-      <c r="B68" s="33">
+      <c r="B68" s="32">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
auf den neuesten Stand gebracht
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/bin/Debug/requirements/Project Board Customization.xlsx
+++ b/Projectboard/Projectboard/bin/Debug/requirements/Project Board Customization.xlsx
@@ -1167,9 +1167,9 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:EI68"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" topLeftCell="B1" colorId="22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="EH22" sqref="EH22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1279,403 +1279,138 @@
       <c r="E17" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="30">
-        <f>Start_Kalender</f>
-        <v>41153</v>
-      </c>
-      <c r="G17" s="30">
-        <v>41183</v>
-      </c>
-      <c r="H17" s="30">
-        <v>41214</v>
-      </c>
-      <c r="I17" s="30">
-        <v>41244</v>
-      </c>
-      <c r="J17" s="30">
-        <v>41275</v>
-      </c>
-      <c r="K17" s="30">
-        <v>41306</v>
-      </c>
-      <c r="L17" s="30">
-        <v>41334</v>
-      </c>
-      <c r="M17" s="30">
-        <v>41365</v>
-      </c>
-      <c r="N17" s="30">
-        <v>41395</v>
-      </c>
-      <c r="O17" s="30">
-        <v>41426</v>
-      </c>
-      <c r="P17" s="30">
-        <v>41456</v>
-      </c>
-      <c r="Q17" s="30">
-        <v>41487</v>
-      </c>
-      <c r="R17" s="30">
-        <v>41518</v>
-      </c>
-      <c r="S17" s="30">
-        <v>41548</v>
-      </c>
-      <c r="T17" s="30">
-        <v>41579</v>
-      </c>
-      <c r="U17" s="30">
-        <v>41609</v>
-      </c>
-      <c r="V17" s="30">
-        <v>41640</v>
-      </c>
-      <c r="W17" s="30">
-        <v>41671</v>
-      </c>
-      <c r="X17" s="30">
-        <v>41699</v>
-      </c>
-      <c r="Y17" s="30">
-        <v>41730</v>
-      </c>
-      <c r="Z17" s="30">
-        <v>41760</v>
-      </c>
-      <c r="AA17" s="30">
-        <v>41791</v>
-      </c>
-      <c r="AB17" s="30">
-        <v>41821</v>
-      </c>
-      <c r="AC17" s="30">
-        <v>41852</v>
-      </c>
-      <c r="AD17" s="30">
-        <v>41883</v>
-      </c>
-      <c r="AE17" s="30">
-        <v>41913</v>
-      </c>
-      <c r="AF17" s="30">
-        <v>41944</v>
-      </c>
-      <c r="AG17" s="30">
-        <v>41974</v>
-      </c>
-      <c r="AH17" s="30">
-        <v>42005</v>
-      </c>
-      <c r="AI17" s="30">
-        <v>42036</v>
-      </c>
-      <c r="AJ17" s="30">
-        <v>42064</v>
-      </c>
-      <c r="AK17" s="30">
-        <v>42095</v>
-      </c>
-      <c r="AL17" s="30">
-        <v>42125</v>
-      </c>
-      <c r="AM17" s="30">
-        <v>42156</v>
-      </c>
-      <c r="AN17" s="30">
-        <v>42186</v>
-      </c>
-      <c r="AO17" s="30">
-        <v>42217</v>
-      </c>
-      <c r="AP17" s="30">
-        <v>42248</v>
-      </c>
-      <c r="AQ17" s="30">
-        <v>42278</v>
-      </c>
-      <c r="AR17" s="30">
-        <v>42309</v>
-      </c>
-      <c r="AS17" s="30">
-        <v>42339</v>
-      </c>
-      <c r="AT17" s="30">
-        <v>42370</v>
-      </c>
-      <c r="AU17" s="30">
-        <v>42401</v>
-      </c>
-      <c r="AV17" s="30">
-        <v>42430</v>
-      </c>
-      <c r="AW17" s="30">
-        <v>42461</v>
-      </c>
-      <c r="AX17" s="30">
-        <v>42491</v>
-      </c>
-      <c r="AY17" s="30">
-        <v>42522</v>
-      </c>
-      <c r="AZ17" s="30">
-        <v>42552</v>
-      </c>
-      <c r="BA17" s="30">
-        <v>42583</v>
-      </c>
-      <c r="BB17" s="30">
-        <v>42614</v>
-      </c>
-      <c r="BC17" s="30">
-        <v>42644</v>
-      </c>
-      <c r="BD17" s="30">
-        <v>42675</v>
-      </c>
-      <c r="BE17" s="30">
-        <v>42705</v>
-      </c>
-      <c r="BF17" s="30">
-        <v>42736</v>
-      </c>
-      <c r="BG17" s="30">
-        <v>42767</v>
-      </c>
-      <c r="BH17" s="30">
-        <v>42795</v>
-      </c>
-      <c r="BI17" s="30">
-        <v>42826</v>
-      </c>
-      <c r="BJ17" s="30">
-        <v>42856</v>
-      </c>
-      <c r="BK17" s="30">
-        <v>42887</v>
-      </c>
-      <c r="BL17" s="30">
-        <v>42917</v>
-      </c>
-      <c r="BM17" s="30">
-        <v>42948</v>
-      </c>
-      <c r="BN17" s="30">
-        <v>42979</v>
-      </c>
-      <c r="BO17" s="30">
-        <v>43009</v>
-      </c>
-      <c r="BP17" s="30">
-        <v>43040</v>
-      </c>
-      <c r="BQ17" s="30">
-        <v>43070</v>
-      </c>
-      <c r="BR17" s="30">
-        <v>43101</v>
-      </c>
-      <c r="BS17" s="30">
-        <v>43132</v>
-      </c>
-      <c r="BT17" s="30">
-        <v>43160</v>
-      </c>
-      <c r="BU17" s="30">
-        <v>43191</v>
-      </c>
-      <c r="BV17" s="30">
-        <v>43221</v>
-      </c>
-      <c r="BW17" s="30">
-        <v>43252</v>
-      </c>
-      <c r="BX17" s="30">
-        <v>43282</v>
-      </c>
-      <c r="BY17" s="30">
-        <v>43313</v>
-      </c>
-      <c r="BZ17" s="30">
-        <v>43344</v>
-      </c>
-      <c r="CA17" s="30">
-        <v>43374</v>
-      </c>
-      <c r="CB17" s="30">
-        <v>43405</v>
-      </c>
-      <c r="CC17" s="30">
-        <v>43435</v>
-      </c>
-      <c r="CD17" s="30">
-        <v>43466</v>
-      </c>
-      <c r="CE17" s="30">
-        <v>43497</v>
-      </c>
-      <c r="CF17" s="30">
-        <v>43525</v>
-      </c>
-      <c r="CG17" s="30">
-        <v>43556</v>
-      </c>
-      <c r="CH17" s="30">
-        <v>43586</v>
-      </c>
-      <c r="CI17" s="30">
-        <v>43617</v>
-      </c>
-      <c r="CJ17" s="30">
-        <v>43647</v>
-      </c>
-      <c r="CK17" s="30">
-        <v>43678</v>
-      </c>
-      <c r="CL17" s="30">
-        <v>43709</v>
-      </c>
-      <c r="CM17" s="30">
-        <v>43739</v>
-      </c>
-      <c r="CN17" s="30">
-        <v>43770</v>
-      </c>
-      <c r="CO17" s="30">
-        <v>43800</v>
-      </c>
-      <c r="CP17" s="30">
-        <v>43831</v>
-      </c>
-      <c r="CQ17" s="30">
-        <v>43862</v>
-      </c>
-      <c r="CR17" s="30">
-        <v>43891</v>
-      </c>
-      <c r="CS17" s="30">
-        <v>43922</v>
-      </c>
-      <c r="CT17" s="30">
-        <v>43952</v>
-      </c>
-      <c r="CU17" s="30">
-        <v>43983</v>
-      </c>
-      <c r="CV17" s="30">
-        <v>44013</v>
-      </c>
-      <c r="CW17" s="30">
-        <v>44044</v>
-      </c>
-      <c r="CX17" s="30">
-        <v>44075</v>
-      </c>
-      <c r="CY17" s="30">
-        <v>44105</v>
-      </c>
-      <c r="CZ17" s="30">
-        <v>44136</v>
-      </c>
-      <c r="DA17" s="30">
-        <v>44166</v>
-      </c>
-      <c r="DB17" s="30">
-        <v>44197</v>
-      </c>
-      <c r="DC17" s="30">
-        <v>44228</v>
-      </c>
-      <c r="DD17" s="30">
-        <v>44256</v>
-      </c>
-      <c r="DE17" s="30">
-        <v>44287</v>
-      </c>
-      <c r="DF17" s="30">
-        <v>44317</v>
-      </c>
-      <c r="DG17" s="30">
-        <v>44348</v>
-      </c>
-      <c r="DH17" s="30">
-        <v>44378</v>
-      </c>
-      <c r="DI17" s="30">
-        <v>44409</v>
-      </c>
-      <c r="DJ17" s="30">
-        <v>44440</v>
-      </c>
-      <c r="DK17" s="30">
-        <v>44470</v>
-      </c>
-      <c r="DL17" s="30">
-        <v>44501</v>
-      </c>
-      <c r="DM17" s="30">
-        <v>44531</v>
-      </c>
-      <c r="DN17" s="30">
-        <v>44562</v>
-      </c>
-      <c r="DO17" s="30">
-        <v>44593</v>
-      </c>
-      <c r="DP17" s="30">
-        <v>44621</v>
-      </c>
-      <c r="DQ17" s="30">
-        <v>44652</v>
-      </c>
-      <c r="DR17" s="30">
-        <v>44682</v>
-      </c>
-      <c r="DS17" s="30">
-        <v>44713</v>
-      </c>
-      <c r="DT17" s="30">
-        <v>44743</v>
-      </c>
-      <c r="DU17" s="30">
-        <v>44774</v>
-      </c>
-      <c r="DV17" s="30">
-        <v>44805</v>
-      </c>
-      <c r="DW17" s="30">
-        <v>44835</v>
-      </c>
-      <c r="DX17" s="30">
-        <v>44866</v>
-      </c>
-      <c r="DY17" s="30">
-        <v>44896</v>
-      </c>
-      <c r="DZ17" s="30">
-        <v>44927</v>
-      </c>
-      <c r="EA17" s="30">
-        <v>44958</v>
-      </c>
-      <c r="EB17" s="30">
-        <v>44986</v>
-      </c>
-      <c r="EC17" s="30">
-        <v>45017</v>
-      </c>
-      <c r="ED17" s="30">
-        <v>45047</v>
-      </c>
-      <c r="EE17" s="30">
-        <v>45078</v>
-      </c>
-      <c r="EF17" s="30">
-        <v>45108</v>
-      </c>
-      <c r="EG17" s="30">
-        <v>45139</v>
-      </c>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="30"/>
+      <c r="AA17" s="30"/>
+      <c r="AB17" s="30"/>
+      <c r="AC17" s="30"/>
+      <c r="AD17" s="30"/>
+      <c r="AE17" s="30"/>
+      <c r="AF17" s="30"/>
+      <c r="AG17" s="30"/>
+      <c r="AH17" s="30"/>
+      <c r="AI17" s="30"/>
+      <c r="AJ17" s="30"/>
+      <c r="AK17" s="30"/>
+      <c r="AL17" s="30"/>
+      <c r="AM17" s="30"/>
+      <c r="AN17" s="30"/>
+      <c r="AO17" s="30"/>
+      <c r="AP17" s="30"/>
+      <c r="AQ17" s="30"/>
+      <c r="AR17" s="30"/>
+      <c r="AS17" s="30"/>
+      <c r="AT17" s="30"/>
+      <c r="AU17" s="30"/>
+      <c r="AV17" s="30"/>
+      <c r="AW17" s="30"/>
+      <c r="AX17" s="30"/>
+      <c r="AY17" s="30"/>
+      <c r="AZ17" s="30"/>
+      <c r="BA17" s="30"/>
+      <c r="BB17" s="30"/>
+      <c r="BC17" s="30"/>
+      <c r="BD17" s="30"/>
+      <c r="BE17" s="30"/>
+      <c r="BF17" s="30"/>
+      <c r="BG17" s="30"/>
+      <c r="BH17" s="30"/>
+      <c r="BI17" s="30"/>
+      <c r="BJ17" s="30"/>
+      <c r="BK17" s="30"/>
+      <c r="BL17" s="30"/>
+      <c r="BM17" s="30"/>
+      <c r="BN17" s="30"/>
+      <c r="BO17" s="30"/>
+      <c r="BP17" s="30"/>
+      <c r="BQ17" s="30"/>
+      <c r="BR17" s="30"/>
+      <c r="BS17" s="30"/>
+      <c r="BT17" s="30"/>
+      <c r="BU17" s="30"/>
+      <c r="BV17" s="30"/>
+      <c r="BW17" s="30"/>
+      <c r="BX17" s="30"/>
+      <c r="BY17" s="30"/>
+      <c r="BZ17" s="30"/>
+      <c r="CA17" s="30"/>
+      <c r="CB17" s="30"/>
+      <c r="CC17" s="30"/>
+      <c r="CD17" s="30"/>
+      <c r="CE17" s="30"/>
+      <c r="CF17" s="30"/>
+      <c r="CG17" s="30"/>
+      <c r="CH17" s="30"/>
+      <c r="CI17" s="30"/>
+      <c r="CJ17" s="30"/>
+      <c r="CK17" s="30"/>
+      <c r="CL17" s="30"/>
+      <c r="CM17" s="30"/>
+      <c r="CN17" s="30"/>
+      <c r="CO17" s="30"/>
+      <c r="CP17" s="30"/>
+      <c r="CQ17" s="30"/>
+      <c r="CR17" s="30"/>
+      <c r="CS17" s="30"/>
+      <c r="CT17" s="30"/>
+      <c r="CU17" s="30"/>
+      <c r="CV17" s="30"/>
+      <c r="CW17" s="30"/>
+      <c r="CX17" s="30"/>
+      <c r="CY17" s="30"/>
+      <c r="CZ17" s="30"/>
+      <c r="DA17" s="30"/>
+      <c r="DB17" s="30"/>
+      <c r="DC17" s="30"/>
+      <c r="DD17" s="30"/>
+      <c r="DE17" s="30"/>
+      <c r="DF17" s="30"/>
+      <c r="DG17" s="30"/>
+      <c r="DH17" s="30"/>
+      <c r="DI17" s="30"/>
+      <c r="DJ17" s="30"/>
+      <c r="DK17" s="30"/>
+      <c r="DL17" s="30"/>
+      <c r="DM17" s="30"/>
+      <c r="DN17" s="30"/>
+      <c r="DO17" s="30"/>
+      <c r="DP17" s="30"/>
+      <c r="DQ17" s="30"/>
+      <c r="DR17" s="30"/>
+      <c r="DS17" s="30"/>
+      <c r="DT17" s="30"/>
+      <c r="DU17" s="30"/>
+      <c r="DV17" s="30"/>
+      <c r="DW17" s="30"/>
+      <c r="DX17" s="30"/>
+      <c r="DY17" s="30"/>
+      <c r="DZ17" s="30"/>
+      <c r="EA17" s="30"/>
+      <c r="EB17" s="30"/>
+      <c r="EC17" s="30"/>
+      <c r="ED17" s="30"/>
+      <c r="EE17" s="30"/>
+      <c r="EF17" s="30"/>
+      <c r="EG17" s="30"/>
       <c r="EH17" s="30"/>
       <c r="EI17" s="30"/>
     </row>
@@ -1684,521 +1419,10 @@
         <v>12</v>
       </c>
       <c r="C18" s="7">
-        <v>100</v>
+        <v>36</v>
       </c>
       <c r="D18">
         <v>440</v>
-      </c>
-      <c r="F18">
-        <f>C18</f>
-        <v>100</v>
-      </c>
-      <c r="G18">
-        <f t="shared" ref="G18:G23" si="0">F18</f>
-        <v>100</v>
-      </c>
-      <c r="H18">
-        <f t="shared" ref="H18:N23" si="1">G18</f>
-        <v>100</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="O18">
-        <f t="shared" ref="O18:O23" si="2">N18</f>
-        <v>100</v>
-      </c>
-      <c r="P18">
-        <f t="shared" ref="P18:P23" si="3">O18</f>
-        <v>100</v>
-      </c>
-      <c r="Q18">
-        <v>90</v>
-      </c>
-      <c r="R18">
-        <v>100</v>
-      </c>
-      <c r="S18">
-        <v>110</v>
-      </c>
-      <c r="T18">
-        <v>120</v>
-      </c>
-      <c r="U18">
-        <v>70</v>
-      </c>
-      <c r="V18">
-        <v>120</v>
-      </c>
-      <c r="W18">
-        <v>120</v>
-      </c>
-      <c r="X18">
-        <v>110</v>
-      </c>
-      <c r="Y18">
-        <v>110</v>
-      </c>
-      <c r="Z18">
-        <v>110</v>
-      </c>
-      <c r="AA18">
-        <v>110</v>
-      </c>
-      <c r="AB18">
-        <v>110</v>
-      </c>
-      <c r="AC18">
-        <v>110</v>
-      </c>
-      <c r="AD18">
-        <v>110</v>
-      </c>
-      <c r="AE18">
-        <v>110</v>
-      </c>
-      <c r="AF18">
-        <v>110</v>
-      </c>
-      <c r="AG18">
-        <v>110</v>
-      </c>
-      <c r="AH18">
-        <f t="shared" ref="AH18:AH23" si="4">AG18</f>
-        <v>110</v>
-      </c>
-      <c r="AI18">
-        <f t="shared" ref="AI18:AI23" si="5">AH18</f>
-        <v>110</v>
-      </c>
-      <c r="AJ18">
-        <f t="shared" ref="AJ18:AJ23" si="6">AI18</f>
-        <v>110</v>
-      </c>
-      <c r="AK18">
-        <f t="shared" ref="AK18:AK23" si="7">AJ18</f>
-        <v>110</v>
-      </c>
-      <c r="AL18">
-        <f t="shared" ref="AL18:AL23" si="8">AK18</f>
-        <v>110</v>
-      </c>
-      <c r="AM18">
-        <f t="shared" ref="AM18:AM23" si="9">AL18</f>
-        <v>110</v>
-      </c>
-      <c r="AN18">
-        <f t="shared" ref="AN18:AN23" si="10">AM18</f>
-        <v>110</v>
-      </c>
-      <c r="AO18">
-        <f t="shared" ref="AO18:AO23" si="11">AN18</f>
-        <v>110</v>
-      </c>
-      <c r="AP18">
-        <f t="shared" ref="AP18:AP23" si="12">AO18</f>
-        <v>110</v>
-      </c>
-      <c r="AQ18">
-        <f t="shared" ref="AQ18:AQ23" si="13">AP18</f>
-        <v>110</v>
-      </c>
-      <c r="AR18">
-        <f t="shared" ref="AR18:AR23" si="14">AQ18</f>
-        <v>110</v>
-      </c>
-      <c r="AS18">
-        <f t="shared" ref="AS18:AS23" si="15">AR18</f>
-        <v>110</v>
-      </c>
-      <c r="AT18">
-        <f t="shared" ref="AT18:AT23" si="16">AS18</f>
-        <v>110</v>
-      </c>
-      <c r="AU18">
-        <f t="shared" ref="AU18:AU23" si="17">AT18</f>
-        <v>110</v>
-      </c>
-      <c r="AV18">
-        <f t="shared" ref="AV18:AV23" si="18">AU18</f>
-        <v>110</v>
-      </c>
-      <c r="AW18">
-        <f t="shared" ref="AW18:AW23" si="19">AV18</f>
-        <v>110</v>
-      </c>
-      <c r="AX18">
-        <f t="shared" ref="AX18:AX23" si="20">AW18</f>
-        <v>110</v>
-      </c>
-      <c r="AY18">
-        <f t="shared" ref="AY18:AY23" si="21">AX18</f>
-        <v>110</v>
-      </c>
-      <c r="AZ18">
-        <f t="shared" ref="AZ18:AZ23" si="22">AY18</f>
-        <v>110</v>
-      </c>
-      <c r="BA18">
-        <f t="shared" ref="BA18:BA23" si="23">AZ18</f>
-        <v>110</v>
-      </c>
-      <c r="BB18">
-        <f t="shared" ref="BB18:BB23" si="24">BA18</f>
-        <v>110</v>
-      </c>
-      <c r="BC18">
-        <f t="shared" ref="BC18:BC23" si="25">BB18</f>
-        <v>110</v>
-      </c>
-      <c r="BD18">
-        <f t="shared" ref="BD18:BD23" si="26">BC18</f>
-        <v>110</v>
-      </c>
-      <c r="BE18">
-        <f t="shared" ref="BE18:BE23" si="27">BD18</f>
-        <v>110</v>
-      </c>
-      <c r="BF18">
-        <f t="shared" ref="BF18:BF23" si="28">BE18</f>
-        <v>110</v>
-      </c>
-      <c r="BG18">
-        <f t="shared" ref="BG18:BG23" si="29">BF18</f>
-        <v>110</v>
-      </c>
-      <c r="BH18">
-        <f t="shared" ref="BH18:BH23" si="30">BG18</f>
-        <v>110</v>
-      </c>
-      <c r="BI18">
-        <f t="shared" ref="BI18:BI23" si="31">BH18</f>
-        <v>110</v>
-      </c>
-      <c r="BJ18">
-        <f t="shared" ref="BJ18:BJ23" si="32">BI18</f>
-        <v>110</v>
-      </c>
-      <c r="BK18">
-        <f t="shared" ref="BK18:BK23" si="33">BJ18</f>
-        <v>110</v>
-      </c>
-      <c r="BL18">
-        <f t="shared" ref="BL18:BL23" si="34">BK18</f>
-        <v>110</v>
-      </c>
-      <c r="BM18">
-        <f t="shared" ref="BM18:BM23" si="35">BL18</f>
-        <v>110</v>
-      </c>
-      <c r="BN18">
-        <f t="shared" ref="BN18:BN23" si="36">BM18</f>
-        <v>110</v>
-      </c>
-      <c r="BO18">
-        <f t="shared" ref="BO18:BO23" si="37">BN18</f>
-        <v>110</v>
-      </c>
-      <c r="BP18">
-        <f t="shared" ref="BP18:BP23" si="38">BO18</f>
-        <v>110</v>
-      </c>
-      <c r="BQ18">
-        <f t="shared" ref="BQ18:BQ23" si="39">BP18</f>
-        <v>110</v>
-      </c>
-      <c r="BR18">
-        <f t="shared" ref="BR18:BR23" si="40">BQ18</f>
-        <v>110</v>
-      </c>
-      <c r="BS18">
-        <f t="shared" ref="BS18:BS23" si="41">BR18</f>
-        <v>110</v>
-      </c>
-      <c r="BT18">
-        <f t="shared" ref="BT18:BT23" si="42">BS18</f>
-        <v>110</v>
-      </c>
-      <c r="BU18">
-        <f t="shared" ref="BU18:BU23" si="43">BT18</f>
-        <v>110</v>
-      </c>
-      <c r="BV18">
-        <f t="shared" ref="BV18:BV23" si="44">BU18</f>
-        <v>110</v>
-      </c>
-      <c r="BW18">
-        <f t="shared" ref="BW18:BW23" si="45">BV18</f>
-        <v>110</v>
-      </c>
-      <c r="BX18">
-        <f t="shared" ref="BX18:BX23" si="46">BW18</f>
-        <v>110</v>
-      </c>
-      <c r="BY18">
-        <f t="shared" ref="BY18:BY23" si="47">BX18</f>
-        <v>110</v>
-      </c>
-      <c r="BZ18">
-        <f t="shared" ref="BZ18:BZ23" si="48">BY18</f>
-        <v>110</v>
-      </c>
-      <c r="CA18">
-        <f t="shared" ref="CA18:CA23" si="49">BZ18</f>
-        <v>110</v>
-      </c>
-      <c r="CB18">
-        <f t="shared" ref="CB18:CB23" si="50">CA18</f>
-        <v>110</v>
-      </c>
-      <c r="CC18">
-        <f t="shared" ref="CC18:CC23" si="51">CB18</f>
-        <v>110</v>
-      </c>
-      <c r="CD18">
-        <f t="shared" ref="CD18:CD23" si="52">CC18</f>
-        <v>110</v>
-      </c>
-      <c r="CE18">
-        <f t="shared" ref="CE18:CE23" si="53">CD18</f>
-        <v>110</v>
-      </c>
-      <c r="CF18">
-        <f t="shared" ref="CF18:CF23" si="54">CE18</f>
-        <v>110</v>
-      </c>
-      <c r="CG18">
-        <f t="shared" ref="CG18:CG23" si="55">CF18</f>
-        <v>110</v>
-      </c>
-      <c r="CH18">
-        <f t="shared" ref="CH18:CH23" si="56">CG18</f>
-        <v>110</v>
-      </c>
-      <c r="CI18">
-        <f t="shared" ref="CI18:CI23" si="57">CH18</f>
-        <v>110</v>
-      </c>
-      <c r="CJ18">
-        <f t="shared" ref="CJ18:CJ23" si="58">CI18</f>
-        <v>110</v>
-      </c>
-      <c r="CK18">
-        <f t="shared" ref="CK18:CK23" si="59">CJ18</f>
-        <v>110</v>
-      </c>
-      <c r="CL18">
-        <f t="shared" ref="CL18:CL23" si="60">CK18</f>
-        <v>110</v>
-      </c>
-      <c r="CM18">
-        <f t="shared" ref="CM18:CM23" si="61">CL18</f>
-        <v>110</v>
-      </c>
-      <c r="CN18">
-        <f t="shared" ref="CN18:CN23" si="62">CM18</f>
-        <v>110</v>
-      </c>
-      <c r="CO18">
-        <f t="shared" ref="CO18:CO23" si="63">CN18</f>
-        <v>110</v>
-      </c>
-      <c r="CP18">
-        <f t="shared" ref="CP18:CP23" si="64">CO18</f>
-        <v>110</v>
-      </c>
-      <c r="CQ18">
-        <f t="shared" ref="CQ18:CQ23" si="65">CP18</f>
-        <v>110</v>
-      </c>
-      <c r="CR18">
-        <f t="shared" ref="CR18:CR23" si="66">CQ18</f>
-        <v>110</v>
-      </c>
-      <c r="CS18">
-        <f t="shared" ref="CS18:CS23" si="67">CR18</f>
-        <v>110</v>
-      </c>
-      <c r="CT18">
-        <f t="shared" ref="CT18:CT23" si="68">CS18</f>
-        <v>110</v>
-      </c>
-      <c r="CU18">
-        <f t="shared" ref="CU18:CU23" si="69">CT18</f>
-        <v>110</v>
-      </c>
-      <c r="CV18">
-        <f t="shared" ref="CV18:CV23" si="70">CU18</f>
-        <v>110</v>
-      </c>
-      <c r="CW18">
-        <f t="shared" ref="CW18:CW23" si="71">CV18</f>
-        <v>110</v>
-      </c>
-      <c r="CX18">
-        <f t="shared" ref="CX18:CX23" si="72">CW18</f>
-        <v>110</v>
-      </c>
-      <c r="CY18">
-        <f t="shared" ref="CY18:CY23" si="73">CX18</f>
-        <v>110</v>
-      </c>
-      <c r="CZ18">
-        <f t="shared" ref="CZ18:CZ23" si="74">CY18</f>
-        <v>110</v>
-      </c>
-      <c r="DA18">
-        <f t="shared" ref="DA18:DA23" si="75">CZ18</f>
-        <v>110</v>
-      </c>
-      <c r="DB18">
-        <f t="shared" ref="DB18:DB23" si="76">DA18</f>
-        <v>110</v>
-      </c>
-      <c r="DC18">
-        <f t="shared" ref="DC18:DC23" si="77">DB18</f>
-        <v>110</v>
-      </c>
-      <c r="DD18">
-        <f t="shared" ref="DD18:DD23" si="78">DC18</f>
-        <v>110</v>
-      </c>
-      <c r="DE18">
-        <f t="shared" ref="DE18:DE23" si="79">DD18</f>
-        <v>110</v>
-      </c>
-      <c r="DF18">
-        <f t="shared" ref="DF18:DF23" si="80">DE18</f>
-        <v>110</v>
-      </c>
-      <c r="DG18">
-        <f t="shared" ref="DG18:DG23" si="81">DF18</f>
-        <v>110</v>
-      </c>
-      <c r="DH18">
-        <f t="shared" ref="DH18:DH23" si="82">DG18</f>
-        <v>110</v>
-      </c>
-      <c r="DI18">
-        <f t="shared" ref="DI18:DI23" si="83">DH18</f>
-        <v>110</v>
-      </c>
-      <c r="DJ18">
-        <f t="shared" ref="DJ18:DJ23" si="84">DI18</f>
-        <v>110</v>
-      </c>
-      <c r="DK18">
-        <f t="shared" ref="DK18:DK23" si="85">DJ18</f>
-        <v>110</v>
-      </c>
-      <c r="DL18">
-        <f t="shared" ref="DL18:DL23" si="86">DK18</f>
-        <v>110</v>
-      </c>
-      <c r="DM18">
-        <f t="shared" ref="DM18:DM23" si="87">DL18</f>
-        <v>110</v>
-      </c>
-      <c r="DN18">
-        <f t="shared" ref="DN18:DN23" si="88">DM18</f>
-        <v>110</v>
-      </c>
-      <c r="DO18">
-        <f t="shared" ref="DO18:DO23" si="89">DN18</f>
-        <v>110</v>
-      </c>
-      <c r="DP18">
-        <f t="shared" ref="DP18:DP23" si="90">DO18</f>
-        <v>110</v>
-      </c>
-      <c r="DQ18">
-        <f t="shared" ref="DQ18:DQ23" si="91">DP18</f>
-        <v>110</v>
-      </c>
-      <c r="DR18">
-        <f t="shared" ref="DR18:DR23" si="92">DQ18</f>
-        <v>110</v>
-      </c>
-      <c r="DS18">
-        <f t="shared" ref="DS18:DS23" si="93">DR18</f>
-        <v>110</v>
-      </c>
-      <c r="DT18">
-        <f t="shared" ref="DT18:DT23" si="94">DS18</f>
-        <v>110</v>
-      </c>
-      <c r="DU18">
-        <f t="shared" ref="DU18:DU23" si="95">DT18</f>
-        <v>110</v>
-      </c>
-      <c r="DV18">
-        <f t="shared" ref="DV18:DV23" si="96">DU18</f>
-        <v>110</v>
-      </c>
-      <c r="DW18">
-        <f t="shared" ref="DW18:DW23" si="97">DV18</f>
-        <v>110</v>
-      </c>
-      <c r="DX18">
-        <f t="shared" ref="DX18:DX23" si="98">DW18</f>
-        <v>110</v>
-      </c>
-      <c r="DY18">
-        <f t="shared" ref="DY18:DY23" si="99">DX18</f>
-        <v>110</v>
-      </c>
-      <c r="DZ18">
-        <f t="shared" ref="DZ18:DZ23" si="100">DY18</f>
-        <v>110</v>
-      </c>
-      <c r="EA18">
-        <f t="shared" ref="EA18:EA23" si="101">DZ18</f>
-        <v>110</v>
-      </c>
-      <c r="EB18">
-        <f t="shared" ref="EB18:EB23" si="102">EA18</f>
-        <v>110</v>
-      </c>
-      <c r="EC18">
-        <f t="shared" ref="EC18:EC23" si="103">EB18</f>
-        <v>110</v>
-      </c>
-      <c r="ED18">
-        <f t="shared" ref="ED18:ED23" si="104">EC18</f>
-        <v>110</v>
-      </c>
-      <c r="EE18">
-        <f t="shared" ref="EE18:EE23" si="105">ED18</f>
-        <v>110</v>
-      </c>
-      <c r="EF18">
-        <f t="shared" ref="EF18:EF23" si="106">EE18</f>
-        <v>110</v>
-      </c>
-      <c r="EG18">
-        <f t="shared" ref="EG18:EG23" si="107">EF18</f>
-        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:139" x14ac:dyDescent="0.3">
@@ -2211,534 +1435,6 @@
       <c r="D19">
         <v>370</v>
       </c>
-      <c r="F19">
-        <f>$C19</f>
-        <v>30</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" ref="Q19" si="108">P19</f>
-        <v>30</v>
-      </c>
-      <c r="R19">
-        <f t="shared" ref="R19" si="109">Q19</f>
-        <v>30</v>
-      </c>
-      <c r="S19">
-        <f t="shared" ref="S19" si="110">R19</f>
-        <v>30</v>
-      </c>
-      <c r="T19">
-        <f t="shared" ref="T19" si="111">S19</f>
-        <v>30</v>
-      </c>
-      <c r="U19">
-        <f t="shared" ref="U19" si="112">T19</f>
-        <v>30</v>
-      </c>
-      <c r="V19">
-        <f t="shared" ref="V19" si="113">U19</f>
-        <v>30</v>
-      </c>
-      <c r="W19">
-        <f t="shared" ref="W19" si="114">V19</f>
-        <v>30</v>
-      </c>
-      <c r="X19">
-        <f t="shared" ref="X19" si="115">W19</f>
-        <v>30</v>
-      </c>
-      <c r="Y19">
-        <f t="shared" ref="Y19" si="116">X19</f>
-        <v>30</v>
-      </c>
-      <c r="Z19">
-        <f t="shared" ref="Z19" si="117">Y19</f>
-        <v>30</v>
-      </c>
-      <c r="AA19">
-        <f t="shared" ref="AA19" si="118">Z19</f>
-        <v>30</v>
-      </c>
-      <c r="AB19">
-        <f t="shared" ref="AB19" si="119">AA19</f>
-        <v>30</v>
-      </c>
-      <c r="AC19">
-        <f t="shared" ref="AC19" si="120">AB19</f>
-        <v>30</v>
-      </c>
-      <c r="AD19">
-        <f t="shared" ref="AD19" si="121">AC19</f>
-        <v>30</v>
-      </c>
-      <c r="AE19">
-        <f t="shared" ref="AE19" si="122">AD19</f>
-        <v>30</v>
-      </c>
-      <c r="AF19">
-        <f t="shared" ref="AF19" si="123">AE19</f>
-        <v>30</v>
-      </c>
-      <c r="AG19">
-        <f t="shared" ref="AG19" si="124">AF19</f>
-        <v>30</v>
-      </c>
-      <c r="AH19">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="AI19">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="AJ19">
-        <f t="shared" si="6"/>
-        <v>30</v>
-      </c>
-      <c r="AK19">
-        <f t="shared" si="7"/>
-        <v>30</v>
-      </c>
-      <c r="AL19">
-        <f t="shared" si="8"/>
-        <v>30</v>
-      </c>
-      <c r="AM19">
-        <f t="shared" si="9"/>
-        <v>30</v>
-      </c>
-      <c r="AN19">
-        <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-      <c r="AO19">
-        <f t="shared" si="11"/>
-        <v>30</v>
-      </c>
-      <c r="AP19">
-        <f t="shared" si="12"/>
-        <v>30</v>
-      </c>
-      <c r="AQ19">
-        <f t="shared" si="13"/>
-        <v>30</v>
-      </c>
-      <c r="AR19">
-        <f t="shared" si="14"/>
-        <v>30</v>
-      </c>
-      <c r="AS19">
-        <f t="shared" si="15"/>
-        <v>30</v>
-      </c>
-      <c r="AT19">
-        <f t="shared" si="16"/>
-        <v>30</v>
-      </c>
-      <c r="AU19">
-        <f t="shared" si="17"/>
-        <v>30</v>
-      </c>
-      <c r="AV19">
-        <f t="shared" si="18"/>
-        <v>30</v>
-      </c>
-      <c r="AW19">
-        <f t="shared" si="19"/>
-        <v>30</v>
-      </c>
-      <c r="AX19">
-        <f t="shared" si="20"/>
-        <v>30</v>
-      </c>
-      <c r="AY19">
-        <f t="shared" si="21"/>
-        <v>30</v>
-      </c>
-      <c r="AZ19">
-        <f t="shared" si="22"/>
-        <v>30</v>
-      </c>
-      <c r="BA19">
-        <f t="shared" si="23"/>
-        <v>30</v>
-      </c>
-      <c r="BB19">
-        <f t="shared" si="24"/>
-        <v>30</v>
-      </c>
-      <c r="BC19">
-        <f t="shared" si="25"/>
-        <v>30</v>
-      </c>
-      <c r="BD19">
-        <f t="shared" si="26"/>
-        <v>30</v>
-      </c>
-      <c r="BE19">
-        <f t="shared" si="27"/>
-        <v>30</v>
-      </c>
-      <c r="BF19">
-        <f t="shared" si="28"/>
-        <v>30</v>
-      </c>
-      <c r="BG19">
-        <f t="shared" si="29"/>
-        <v>30</v>
-      </c>
-      <c r="BH19">
-        <f t="shared" si="30"/>
-        <v>30</v>
-      </c>
-      <c r="BI19">
-        <f t="shared" si="31"/>
-        <v>30</v>
-      </c>
-      <c r="BJ19">
-        <f t="shared" si="32"/>
-        <v>30</v>
-      </c>
-      <c r="BK19">
-        <f t="shared" si="33"/>
-        <v>30</v>
-      </c>
-      <c r="BL19">
-        <f t="shared" si="34"/>
-        <v>30</v>
-      </c>
-      <c r="BM19">
-        <f t="shared" si="35"/>
-        <v>30</v>
-      </c>
-      <c r="BN19">
-        <f t="shared" si="36"/>
-        <v>30</v>
-      </c>
-      <c r="BO19">
-        <f t="shared" si="37"/>
-        <v>30</v>
-      </c>
-      <c r="BP19">
-        <f t="shared" si="38"/>
-        <v>30</v>
-      </c>
-      <c r="BQ19">
-        <f t="shared" si="39"/>
-        <v>30</v>
-      </c>
-      <c r="BR19">
-        <f t="shared" si="40"/>
-        <v>30</v>
-      </c>
-      <c r="BS19">
-        <f t="shared" si="41"/>
-        <v>30</v>
-      </c>
-      <c r="BT19">
-        <f t="shared" si="42"/>
-        <v>30</v>
-      </c>
-      <c r="BU19">
-        <f t="shared" si="43"/>
-        <v>30</v>
-      </c>
-      <c r="BV19">
-        <f t="shared" si="44"/>
-        <v>30</v>
-      </c>
-      <c r="BW19">
-        <f t="shared" si="45"/>
-        <v>30</v>
-      </c>
-      <c r="BX19">
-        <f t="shared" si="46"/>
-        <v>30</v>
-      </c>
-      <c r="BY19">
-        <f t="shared" si="47"/>
-        <v>30</v>
-      </c>
-      <c r="BZ19">
-        <f t="shared" si="48"/>
-        <v>30</v>
-      </c>
-      <c r="CA19">
-        <f t="shared" si="49"/>
-        <v>30</v>
-      </c>
-      <c r="CB19">
-        <f t="shared" si="50"/>
-        <v>30</v>
-      </c>
-      <c r="CC19">
-        <f t="shared" si="51"/>
-        <v>30</v>
-      </c>
-      <c r="CD19">
-        <f t="shared" si="52"/>
-        <v>30</v>
-      </c>
-      <c r="CE19">
-        <f t="shared" si="53"/>
-        <v>30</v>
-      </c>
-      <c r="CF19">
-        <f t="shared" si="54"/>
-        <v>30</v>
-      </c>
-      <c r="CG19">
-        <f t="shared" si="55"/>
-        <v>30</v>
-      </c>
-      <c r="CH19">
-        <f t="shared" si="56"/>
-        <v>30</v>
-      </c>
-      <c r="CI19">
-        <f t="shared" si="57"/>
-        <v>30</v>
-      </c>
-      <c r="CJ19">
-        <f t="shared" si="58"/>
-        <v>30</v>
-      </c>
-      <c r="CK19">
-        <f t="shared" si="59"/>
-        <v>30</v>
-      </c>
-      <c r="CL19">
-        <f t="shared" si="60"/>
-        <v>30</v>
-      </c>
-      <c r="CM19">
-        <f t="shared" si="61"/>
-        <v>30</v>
-      </c>
-      <c r="CN19">
-        <f t="shared" si="62"/>
-        <v>30</v>
-      </c>
-      <c r="CO19">
-        <f t="shared" si="63"/>
-        <v>30</v>
-      </c>
-      <c r="CP19">
-        <f t="shared" si="64"/>
-        <v>30</v>
-      </c>
-      <c r="CQ19">
-        <f t="shared" si="65"/>
-        <v>30</v>
-      </c>
-      <c r="CR19">
-        <f t="shared" si="66"/>
-        <v>30</v>
-      </c>
-      <c r="CS19">
-        <f t="shared" si="67"/>
-        <v>30</v>
-      </c>
-      <c r="CT19">
-        <f t="shared" si="68"/>
-        <v>30</v>
-      </c>
-      <c r="CU19">
-        <f t="shared" si="69"/>
-        <v>30</v>
-      </c>
-      <c r="CV19">
-        <f t="shared" si="70"/>
-        <v>30</v>
-      </c>
-      <c r="CW19">
-        <f t="shared" si="71"/>
-        <v>30</v>
-      </c>
-      <c r="CX19">
-        <f t="shared" si="72"/>
-        <v>30</v>
-      </c>
-      <c r="CY19">
-        <f t="shared" si="73"/>
-        <v>30</v>
-      </c>
-      <c r="CZ19">
-        <f t="shared" si="74"/>
-        <v>30</v>
-      </c>
-      <c r="DA19">
-        <f t="shared" si="75"/>
-        <v>30</v>
-      </c>
-      <c r="DB19">
-        <f t="shared" si="76"/>
-        <v>30</v>
-      </c>
-      <c r="DC19">
-        <f t="shared" si="77"/>
-        <v>30</v>
-      </c>
-      <c r="DD19">
-        <f t="shared" si="78"/>
-        <v>30</v>
-      </c>
-      <c r="DE19">
-        <f t="shared" si="79"/>
-        <v>30</v>
-      </c>
-      <c r="DF19">
-        <f t="shared" si="80"/>
-        <v>30</v>
-      </c>
-      <c r="DG19">
-        <f t="shared" si="81"/>
-        <v>30</v>
-      </c>
-      <c r="DH19">
-        <f t="shared" si="82"/>
-        <v>30</v>
-      </c>
-      <c r="DI19">
-        <f t="shared" si="83"/>
-        <v>30</v>
-      </c>
-      <c r="DJ19">
-        <f t="shared" si="84"/>
-        <v>30</v>
-      </c>
-      <c r="DK19">
-        <f t="shared" si="85"/>
-        <v>30</v>
-      </c>
-      <c r="DL19">
-        <f t="shared" si="86"/>
-        <v>30</v>
-      </c>
-      <c r="DM19">
-        <f t="shared" si="87"/>
-        <v>30</v>
-      </c>
-      <c r="DN19">
-        <f t="shared" si="88"/>
-        <v>30</v>
-      </c>
-      <c r="DO19">
-        <f t="shared" si="89"/>
-        <v>30</v>
-      </c>
-      <c r="DP19">
-        <f t="shared" si="90"/>
-        <v>30</v>
-      </c>
-      <c r="DQ19">
-        <f t="shared" si="91"/>
-        <v>30</v>
-      </c>
-      <c r="DR19">
-        <f t="shared" si="92"/>
-        <v>30</v>
-      </c>
-      <c r="DS19">
-        <f t="shared" si="93"/>
-        <v>30</v>
-      </c>
-      <c r="DT19">
-        <f t="shared" si="94"/>
-        <v>30</v>
-      </c>
-      <c r="DU19">
-        <f t="shared" si="95"/>
-        <v>30</v>
-      </c>
-      <c r="DV19">
-        <f t="shared" si="96"/>
-        <v>30</v>
-      </c>
-      <c r="DW19">
-        <f t="shared" si="97"/>
-        <v>30</v>
-      </c>
-      <c r="DX19">
-        <f t="shared" si="98"/>
-        <v>30</v>
-      </c>
-      <c r="DY19">
-        <f t="shared" si="99"/>
-        <v>30</v>
-      </c>
-      <c r="DZ19">
-        <f t="shared" si="100"/>
-        <v>30</v>
-      </c>
-      <c r="EA19">
-        <f t="shared" si="101"/>
-        <v>30</v>
-      </c>
-      <c r="EB19">
-        <f t="shared" si="102"/>
-        <v>30</v>
-      </c>
-      <c r="EC19">
-        <f t="shared" si="103"/>
-        <v>30</v>
-      </c>
-      <c r="ED19">
-        <f t="shared" si="104"/>
-        <v>30</v>
-      </c>
-      <c r="EE19">
-        <f t="shared" si="105"/>
-        <v>30</v>
-      </c>
-      <c r="EF19">
-        <f t="shared" si="106"/>
-        <v>30</v>
-      </c>
-      <c r="EG19">
-        <f t="shared" si="107"/>
-        <v>30</v>
-      </c>
     </row>
     <row r="20" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B20" s="28" t="s">
@@ -2750,517 +1446,6 @@
       <c r="D20">
         <v>370</v>
       </c>
-      <c r="F20">
-        <f>$C20</f>
-        <v>60</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="H20">
-        <f>G20</f>
-        <v>60</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="Q20">
-        <v>64</v>
-      </c>
-      <c r="R20">
-        <v>65</v>
-      </c>
-      <c r="S20">
-        <v>65</v>
-      </c>
-      <c r="T20">
-        <v>65</v>
-      </c>
-      <c r="U20">
-        <v>48</v>
-      </c>
-      <c r="V20">
-        <v>64</v>
-      </c>
-      <c r="W20">
-        <v>58</v>
-      </c>
-      <c r="X20">
-        <v>58</v>
-      </c>
-      <c r="Y20">
-        <v>64</v>
-      </c>
-      <c r="Z20">
-        <v>64</v>
-      </c>
-      <c r="AA20">
-        <v>64</v>
-      </c>
-      <c r="AB20">
-        <v>64</v>
-      </c>
-      <c r="AC20">
-        <v>47</v>
-      </c>
-      <c r="AD20">
-        <v>42</v>
-      </c>
-      <c r="AE20">
-        <v>64</v>
-      </c>
-      <c r="AF20">
-        <v>64</v>
-      </c>
-      <c r="AG20">
-        <v>64</v>
-      </c>
-      <c r="AH20">
-        <f t="shared" si="4"/>
-        <v>64</v>
-      </c>
-      <c r="AI20">
-        <f t="shared" si="5"/>
-        <v>64</v>
-      </c>
-      <c r="AJ20">
-        <f t="shared" si="6"/>
-        <v>64</v>
-      </c>
-      <c r="AK20">
-        <f t="shared" si="7"/>
-        <v>64</v>
-      </c>
-      <c r="AL20">
-        <f t="shared" si="8"/>
-        <v>64</v>
-      </c>
-      <c r="AM20">
-        <f t="shared" si="9"/>
-        <v>64</v>
-      </c>
-      <c r="AN20">
-        <f t="shared" si="10"/>
-        <v>64</v>
-      </c>
-      <c r="AO20">
-        <f t="shared" si="11"/>
-        <v>64</v>
-      </c>
-      <c r="AP20">
-        <f t="shared" si="12"/>
-        <v>64</v>
-      </c>
-      <c r="AQ20">
-        <f t="shared" si="13"/>
-        <v>64</v>
-      </c>
-      <c r="AR20">
-        <f t="shared" si="14"/>
-        <v>64</v>
-      </c>
-      <c r="AS20">
-        <f t="shared" si="15"/>
-        <v>64</v>
-      </c>
-      <c r="AT20">
-        <f t="shared" si="16"/>
-        <v>64</v>
-      </c>
-      <c r="AU20">
-        <f t="shared" si="17"/>
-        <v>64</v>
-      </c>
-      <c r="AV20">
-        <f t="shared" si="18"/>
-        <v>64</v>
-      </c>
-      <c r="AW20">
-        <f t="shared" si="19"/>
-        <v>64</v>
-      </c>
-      <c r="AX20">
-        <f t="shared" si="20"/>
-        <v>64</v>
-      </c>
-      <c r="AY20">
-        <f t="shared" si="21"/>
-        <v>64</v>
-      </c>
-      <c r="AZ20">
-        <f t="shared" si="22"/>
-        <v>64</v>
-      </c>
-      <c r="BA20">
-        <f t="shared" si="23"/>
-        <v>64</v>
-      </c>
-      <c r="BB20">
-        <f t="shared" si="24"/>
-        <v>64</v>
-      </c>
-      <c r="BC20">
-        <f t="shared" si="25"/>
-        <v>64</v>
-      </c>
-      <c r="BD20">
-        <f t="shared" si="26"/>
-        <v>64</v>
-      </c>
-      <c r="BE20">
-        <f t="shared" si="27"/>
-        <v>64</v>
-      </c>
-      <c r="BF20">
-        <f t="shared" si="28"/>
-        <v>64</v>
-      </c>
-      <c r="BG20">
-        <f t="shared" si="29"/>
-        <v>64</v>
-      </c>
-      <c r="BH20">
-        <f t="shared" si="30"/>
-        <v>64</v>
-      </c>
-      <c r="BI20">
-        <f t="shared" si="31"/>
-        <v>64</v>
-      </c>
-      <c r="BJ20">
-        <f t="shared" si="32"/>
-        <v>64</v>
-      </c>
-      <c r="BK20">
-        <f t="shared" si="33"/>
-        <v>64</v>
-      </c>
-      <c r="BL20">
-        <f t="shared" si="34"/>
-        <v>64</v>
-      </c>
-      <c r="BM20">
-        <f t="shared" si="35"/>
-        <v>64</v>
-      </c>
-      <c r="BN20">
-        <f t="shared" si="36"/>
-        <v>64</v>
-      </c>
-      <c r="BO20">
-        <f t="shared" si="37"/>
-        <v>64</v>
-      </c>
-      <c r="BP20">
-        <f t="shared" si="38"/>
-        <v>64</v>
-      </c>
-      <c r="BQ20">
-        <f t="shared" si="39"/>
-        <v>64</v>
-      </c>
-      <c r="BR20">
-        <f t="shared" si="40"/>
-        <v>64</v>
-      </c>
-      <c r="BS20">
-        <f t="shared" si="41"/>
-        <v>64</v>
-      </c>
-      <c r="BT20">
-        <f t="shared" si="42"/>
-        <v>64</v>
-      </c>
-      <c r="BU20">
-        <f t="shared" si="43"/>
-        <v>64</v>
-      </c>
-      <c r="BV20">
-        <f t="shared" si="44"/>
-        <v>64</v>
-      </c>
-      <c r="BW20">
-        <f t="shared" si="45"/>
-        <v>64</v>
-      </c>
-      <c r="BX20">
-        <f t="shared" si="46"/>
-        <v>64</v>
-      </c>
-      <c r="BY20">
-        <f t="shared" si="47"/>
-        <v>64</v>
-      </c>
-      <c r="BZ20">
-        <f t="shared" si="48"/>
-        <v>64</v>
-      </c>
-      <c r="CA20">
-        <f t="shared" si="49"/>
-        <v>64</v>
-      </c>
-      <c r="CB20">
-        <f t="shared" si="50"/>
-        <v>64</v>
-      </c>
-      <c r="CC20">
-        <f t="shared" si="51"/>
-        <v>64</v>
-      </c>
-      <c r="CD20">
-        <f t="shared" si="52"/>
-        <v>64</v>
-      </c>
-      <c r="CE20">
-        <f t="shared" si="53"/>
-        <v>64</v>
-      </c>
-      <c r="CF20">
-        <f t="shared" si="54"/>
-        <v>64</v>
-      </c>
-      <c r="CG20">
-        <f t="shared" si="55"/>
-        <v>64</v>
-      </c>
-      <c r="CH20">
-        <f t="shared" si="56"/>
-        <v>64</v>
-      </c>
-      <c r="CI20">
-        <f t="shared" si="57"/>
-        <v>64</v>
-      </c>
-      <c r="CJ20">
-        <f t="shared" si="58"/>
-        <v>64</v>
-      </c>
-      <c r="CK20">
-        <f t="shared" si="59"/>
-        <v>64</v>
-      </c>
-      <c r="CL20">
-        <f t="shared" si="60"/>
-        <v>64</v>
-      </c>
-      <c r="CM20">
-        <f t="shared" si="61"/>
-        <v>64</v>
-      </c>
-      <c r="CN20">
-        <f t="shared" si="62"/>
-        <v>64</v>
-      </c>
-      <c r="CO20">
-        <f t="shared" si="63"/>
-        <v>64</v>
-      </c>
-      <c r="CP20">
-        <f t="shared" si="64"/>
-        <v>64</v>
-      </c>
-      <c r="CQ20">
-        <f t="shared" si="65"/>
-        <v>64</v>
-      </c>
-      <c r="CR20">
-        <f t="shared" si="66"/>
-        <v>64</v>
-      </c>
-      <c r="CS20">
-        <f t="shared" si="67"/>
-        <v>64</v>
-      </c>
-      <c r="CT20">
-        <f t="shared" si="68"/>
-        <v>64</v>
-      </c>
-      <c r="CU20">
-        <f t="shared" si="69"/>
-        <v>64</v>
-      </c>
-      <c r="CV20">
-        <f t="shared" si="70"/>
-        <v>64</v>
-      </c>
-      <c r="CW20">
-        <f t="shared" si="71"/>
-        <v>64</v>
-      </c>
-      <c r="CX20">
-        <f t="shared" si="72"/>
-        <v>64</v>
-      </c>
-      <c r="CY20">
-        <f t="shared" si="73"/>
-        <v>64</v>
-      </c>
-      <c r="CZ20">
-        <f t="shared" si="74"/>
-        <v>64</v>
-      </c>
-      <c r="DA20">
-        <f t="shared" si="75"/>
-        <v>64</v>
-      </c>
-      <c r="DB20">
-        <f t="shared" si="76"/>
-        <v>64</v>
-      </c>
-      <c r="DC20">
-        <f t="shared" si="77"/>
-        <v>64</v>
-      </c>
-      <c r="DD20">
-        <f t="shared" si="78"/>
-        <v>64</v>
-      </c>
-      <c r="DE20">
-        <f t="shared" si="79"/>
-        <v>64</v>
-      </c>
-      <c r="DF20">
-        <f t="shared" si="80"/>
-        <v>64</v>
-      </c>
-      <c r="DG20">
-        <f t="shared" si="81"/>
-        <v>64</v>
-      </c>
-      <c r="DH20">
-        <f t="shared" si="82"/>
-        <v>64</v>
-      </c>
-      <c r="DI20">
-        <f t="shared" si="83"/>
-        <v>64</v>
-      </c>
-      <c r="DJ20">
-        <f t="shared" si="84"/>
-        <v>64</v>
-      </c>
-      <c r="DK20">
-        <f t="shared" si="85"/>
-        <v>64</v>
-      </c>
-      <c r="DL20">
-        <f t="shared" si="86"/>
-        <v>64</v>
-      </c>
-      <c r="DM20">
-        <f t="shared" si="87"/>
-        <v>64</v>
-      </c>
-      <c r="DN20">
-        <f t="shared" si="88"/>
-        <v>64</v>
-      </c>
-      <c r="DO20">
-        <f t="shared" si="89"/>
-        <v>64</v>
-      </c>
-      <c r="DP20">
-        <f t="shared" si="90"/>
-        <v>64</v>
-      </c>
-      <c r="DQ20">
-        <f t="shared" si="91"/>
-        <v>64</v>
-      </c>
-      <c r="DR20">
-        <f t="shared" si="92"/>
-        <v>64</v>
-      </c>
-      <c r="DS20">
-        <f t="shared" si="93"/>
-        <v>64</v>
-      </c>
-      <c r="DT20">
-        <f t="shared" si="94"/>
-        <v>64</v>
-      </c>
-      <c r="DU20">
-        <f t="shared" si="95"/>
-        <v>64</v>
-      </c>
-      <c r="DV20">
-        <f t="shared" si="96"/>
-        <v>64</v>
-      </c>
-      <c r="DW20">
-        <f t="shared" si="97"/>
-        <v>64</v>
-      </c>
-      <c r="DX20">
-        <f t="shared" si="98"/>
-        <v>64</v>
-      </c>
-      <c r="DY20">
-        <f t="shared" si="99"/>
-        <v>64</v>
-      </c>
-      <c r="DZ20">
-        <f t="shared" si="100"/>
-        <v>64</v>
-      </c>
-      <c r="EA20">
-        <f t="shared" si="101"/>
-        <v>64</v>
-      </c>
-      <c r="EB20">
-        <f t="shared" si="102"/>
-        <v>64</v>
-      </c>
-      <c r="EC20">
-        <f t="shared" si="103"/>
-        <v>64</v>
-      </c>
-      <c r="ED20">
-        <f t="shared" si="104"/>
-        <v>64</v>
-      </c>
-      <c r="EE20">
-        <f t="shared" si="105"/>
-        <v>64</v>
-      </c>
-      <c r="EF20">
-        <f t="shared" si="106"/>
-        <v>64</v>
-      </c>
-      <c r="EG20">
-        <f t="shared" si="107"/>
-        <v>64</v>
-      </c>
     </row>
     <row r="21" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B21" s="27" t="s">
@@ -3272,517 +1457,6 @@
       <c r="D21">
         <v>420</v>
       </c>
-      <c r="F21">
-        <f>$C21</f>
-        <v>40</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="H21">
-        <f t="shared" ref="H21" si="125">G21</f>
-        <v>40</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="Q21">
-        <v>40</v>
-      </c>
-      <c r="R21">
-        <v>41</v>
-      </c>
-      <c r="S21">
-        <v>41</v>
-      </c>
-      <c r="T21">
-        <v>41</v>
-      </c>
-      <c r="U21">
-        <v>29</v>
-      </c>
-      <c r="V21">
-        <v>40</v>
-      </c>
-      <c r="W21">
-        <v>34</v>
-      </c>
-      <c r="X21">
-        <v>40</v>
-      </c>
-      <c r="Y21">
-        <v>40</v>
-      </c>
-      <c r="Z21">
-        <v>37</v>
-      </c>
-      <c r="AA21">
-        <v>37</v>
-      </c>
-      <c r="AB21">
-        <v>40</v>
-      </c>
-      <c r="AC21">
-        <v>34</v>
-      </c>
-      <c r="AD21">
-        <v>29</v>
-      </c>
-      <c r="AE21">
-        <v>40</v>
-      </c>
-      <c r="AF21">
-        <v>40</v>
-      </c>
-      <c r="AG21">
-        <v>40</v>
-      </c>
-      <c r="AH21">
-        <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="AI21">
-        <f t="shared" si="5"/>
-        <v>40</v>
-      </c>
-      <c r="AJ21">
-        <f t="shared" si="6"/>
-        <v>40</v>
-      </c>
-      <c r="AK21">
-        <f t="shared" si="7"/>
-        <v>40</v>
-      </c>
-      <c r="AL21">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="AM21">
-        <f t="shared" si="9"/>
-        <v>40</v>
-      </c>
-      <c r="AN21">
-        <f t="shared" si="10"/>
-        <v>40</v>
-      </c>
-      <c r="AO21">
-        <f t="shared" si="11"/>
-        <v>40</v>
-      </c>
-      <c r="AP21">
-        <f t="shared" si="12"/>
-        <v>40</v>
-      </c>
-      <c r="AQ21">
-        <f t="shared" si="13"/>
-        <v>40</v>
-      </c>
-      <c r="AR21">
-        <f t="shared" si="14"/>
-        <v>40</v>
-      </c>
-      <c r="AS21">
-        <f t="shared" si="15"/>
-        <v>40</v>
-      </c>
-      <c r="AT21">
-        <f t="shared" si="16"/>
-        <v>40</v>
-      </c>
-      <c r="AU21">
-        <f t="shared" si="17"/>
-        <v>40</v>
-      </c>
-      <c r="AV21">
-        <f t="shared" si="18"/>
-        <v>40</v>
-      </c>
-      <c r="AW21">
-        <f t="shared" si="19"/>
-        <v>40</v>
-      </c>
-      <c r="AX21">
-        <f t="shared" si="20"/>
-        <v>40</v>
-      </c>
-      <c r="AY21">
-        <f t="shared" si="21"/>
-        <v>40</v>
-      </c>
-      <c r="AZ21">
-        <f t="shared" si="22"/>
-        <v>40</v>
-      </c>
-      <c r="BA21">
-        <f t="shared" si="23"/>
-        <v>40</v>
-      </c>
-      <c r="BB21">
-        <f t="shared" si="24"/>
-        <v>40</v>
-      </c>
-      <c r="BC21">
-        <f t="shared" si="25"/>
-        <v>40</v>
-      </c>
-      <c r="BD21">
-        <f t="shared" si="26"/>
-        <v>40</v>
-      </c>
-      <c r="BE21">
-        <f t="shared" si="27"/>
-        <v>40</v>
-      </c>
-      <c r="BF21">
-        <f t="shared" si="28"/>
-        <v>40</v>
-      </c>
-      <c r="BG21">
-        <f t="shared" si="29"/>
-        <v>40</v>
-      </c>
-      <c r="BH21">
-        <f t="shared" si="30"/>
-        <v>40</v>
-      </c>
-      <c r="BI21">
-        <f t="shared" si="31"/>
-        <v>40</v>
-      </c>
-      <c r="BJ21">
-        <f t="shared" si="32"/>
-        <v>40</v>
-      </c>
-      <c r="BK21">
-        <f t="shared" si="33"/>
-        <v>40</v>
-      </c>
-      <c r="BL21">
-        <f t="shared" si="34"/>
-        <v>40</v>
-      </c>
-      <c r="BM21">
-        <f t="shared" si="35"/>
-        <v>40</v>
-      </c>
-      <c r="BN21">
-        <f t="shared" si="36"/>
-        <v>40</v>
-      </c>
-      <c r="BO21">
-        <f t="shared" si="37"/>
-        <v>40</v>
-      </c>
-      <c r="BP21">
-        <f t="shared" si="38"/>
-        <v>40</v>
-      </c>
-      <c r="BQ21">
-        <f t="shared" si="39"/>
-        <v>40</v>
-      </c>
-      <c r="BR21">
-        <f t="shared" si="40"/>
-        <v>40</v>
-      </c>
-      <c r="BS21">
-        <f t="shared" si="41"/>
-        <v>40</v>
-      </c>
-      <c r="BT21">
-        <f t="shared" si="42"/>
-        <v>40</v>
-      </c>
-      <c r="BU21">
-        <f t="shared" si="43"/>
-        <v>40</v>
-      </c>
-      <c r="BV21">
-        <f t="shared" si="44"/>
-        <v>40</v>
-      </c>
-      <c r="BW21">
-        <f t="shared" si="45"/>
-        <v>40</v>
-      </c>
-      <c r="BX21">
-        <f t="shared" si="46"/>
-        <v>40</v>
-      </c>
-      <c r="BY21">
-        <f t="shared" si="47"/>
-        <v>40</v>
-      </c>
-      <c r="BZ21">
-        <f t="shared" si="48"/>
-        <v>40</v>
-      </c>
-      <c r="CA21">
-        <f t="shared" si="49"/>
-        <v>40</v>
-      </c>
-      <c r="CB21">
-        <f t="shared" si="50"/>
-        <v>40</v>
-      </c>
-      <c r="CC21">
-        <f t="shared" si="51"/>
-        <v>40</v>
-      </c>
-      <c r="CD21">
-        <f t="shared" si="52"/>
-        <v>40</v>
-      </c>
-      <c r="CE21">
-        <f t="shared" si="53"/>
-        <v>40</v>
-      </c>
-      <c r="CF21">
-        <f t="shared" si="54"/>
-        <v>40</v>
-      </c>
-      <c r="CG21">
-        <f t="shared" si="55"/>
-        <v>40</v>
-      </c>
-      <c r="CH21">
-        <f t="shared" si="56"/>
-        <v>40</v>
-      </c>
-      <c r="CI21">
-        <f t="shared" si="57"/>
-        <v>40</v>
-      </c>
-      <c r="CJ21">
-        <f t="shared" si="58"/>
-        <v>40</v>
-      </c>
-      <c r="CK21">
-        <f t="shared" si="59"/>
-        <v>40</v>
-      </c>
-      <c r="CL21">
-        <f t="shared" si="60"/>
-        <v>40</v>
-      </c>
-      <c r="CM21">
-        <f t="shared" si="61"/>
-        <v>40</v>
-      </c>
-      <c r="CN21">
-        <f t="shared" si="62"/>
-        <v>40</v>
-      </c>
-      <c r="CO21">
-        <f t="shared" si="63"/>
-        <v>40</v>
-      </c>
-      <c r="CP21">
-        <f t="shared" si="64"/>
-        <v>40</v>
-      </c>
-      <c r="CQ21">
-        <f t="shared" si="65"/>
-        <v>40</v>
-      </c>
-      <c r="CR21">
-        <f t="shared" si="66"/>
-        <v>40</v>
-      </c>
-      <c r="CS21">
-        <f t="shared" si="67"/>
-        <v>40</v>
-      </c>
-      <c r="CT21">
-        <f t="shared" si="68"/>
-        <v>40</v>
-      </c>
-      <c r="CU21">
-        <f t="shared" si="69"/>
-        <v>40</v>
-      </c>
-      <c r="CV21">
-        <f t="shared" si="70"/>
-        <v>40</v>
-      </c>
-      <c r="CW21">
-        <f t="shared" si="71"/>
-        <v>40</v>
-      </c>
-      <c r="CX21">
-        <f t="shared" si="72"/>
-        <v>40</v>
-      </c>
-      <c r="CY21">
-        <f t="shared" si="73"/>
-        <v>40</v>
-      </c>
-      <c r="CZ21">
-        <f t="shared" si="74"/>
-        <v>40</v>
-      </c>
-      <c r="DA21">
-        <f t="shared" si="75"/>
-        <v>40</v>
-      </c>
-      <c r="DB21">
-        <f t="shared" si="76"/>
-        <v>40</v>
-      </c>
-      <c r="DC21">
-        <f t="shared" si="77"/>
-        <v>40</v>
-      </c>
-      <c r="DD21">
-        <f t="shared" si="78"/>
-        <v>40</v>
-      </c>
-      <c r="DE21">
-        <f t="shared" si="79"/>
-        <v>40</v>
-      </c>
-      <c r="DF21">
-        <f t="shared" si="80"/>
-        <v>40</v>
-      </c>
-      <c r="DG21">
-        <f t="shared" si="81"/>
-        <v>40</v>
-      </c>
-      <c r="DH21">
-        <f t="shared" si="82"/>
-        <v>40</v>
-      </c>
-      <c r="DI21">
-        <f t="shared" si="83"/>
-        <v>40</v>
-      </c>
-      <c r="DJ21">
-        <f t="shared" si="84"/>
-        <v>40</v>
-      </c>
-      <c r="DK21">
-        <f t="shared" si="85"/>
-        <v>40</v>
-      </c>
-      <c r="DL21">
-        <f t="shared" si="86"/>
-        <v>40</v>
-      </c>
-      <c r="DM21">
-        <f t="shared" si="87"/>
-        <v>40</v>
-      </c>
-      <c r="DN21">
-        <f t="shared" si="88"/>
-        <v>40</v>
-      </c>
-      <c r="DO21">
-        <f t="shared" si="89"/>
-        <v>40</v>
-      </c>
-      <c r="DP21">
-        <f t="shared" si="90"/>
-        <v>40</v>
-      </c>
-      <c r="DQ21">
-        <f t="shared" si="91"/>
-        <v>40</v>
-      </c>
-      <c r="DR21">
-        <f t="shared" si="92"/>
-        <v>40</v>
-      </c>
-      <c r="DS21">
-        <f t="shared" si="93"/>
-        <v>40</v>
-      </c>
-      <c r="DT21">
-        <f t="shared" si="94"/>
-        <v>40</v>
-      </c>
-      <c r="DU21">
-        <f t="shared" si="95"/>
-        <v>40</v>
-      </c>
-      <c r="DV21">
-        <f t="shared" si="96"/>
-        <v>40</v>
-      </c>
-      <c r="DW21">
-        <f t="shared" si="97"/>
-        <v>40</v>
-      </c>
-      <c r="DX21">
-        <f t="shared" si="98"/>
-        <v>40</v>
-      </c>
-      <c r="DY21">
-        <f t="shared" si="99"/>
-        <v>40</v>
-      </c>
-      <c r="DZ21">
-        <f t="shared" si="100"/>
-        <v>40</v>
-      </c>
-      <c r="EA21">
-        <f t="shared" si="101"/>
-        <v>40</v>
-      </c>
-      <c r="EB21">
-        <f t="shared" si="102"/>
-        <v>40</v>
-      </c>
-      <c r="EC21">
-        <f t="shared" si="103"/>
-        <v>40</v>
-      </c>
-      <c r="ED21">
-        <f t="shared" si="104"/>
-        <v>40</v>
-      </c>
-      <c r="EE21">
-        <f t="shared" si="105"/>
-        <v>40</v>
-      </c>
-      <c r="EF21">
-        <f t="shared" si="106"/>
-        <v>40</v>
-      </c>
-      <c r="EG21">
-        <f t="shared" si="107"/>
-        <v>40</v>
-      </c>
     </row>
     <row r="22" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B22" s="29" t="s">
@@ -3794,517 +1468,6 @@
       <c r="D22">
         <v>330</v>
       </c>
-      <c r="F22">
-        <f t="shared" ref="F22" si="126">$C22</f>
-        <v>140</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="H22">
-        <f t="shared" ref="H22" si="127">G22</f>
-        <v>140</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
-        <v>140</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="1"/>
-        <v>140</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="1"/>
-        <v>140</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="1"/>
-        <v>140</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="1"/>
-        <v>140</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="1"/>
-        <v>140</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="2"/>
-        <v>140</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="3"/>
-        <v>140</v>
-      </c>
-      <c r="Q22">
-        <v>144</v>
-      </c>
-      <c r="R22">
-        <v>140</v>
-      </c>
-      <c r="S22">
-        <v>144</v>
-      </c>
-      <c r="T22">
-        <v>144</v>
-      </c>
-      <c r="U22">
-        <v>126</v>
-      </c>
-      <c r="V22">
-        <v>132</v>
-      </c>
-      <c r="W22">
-        <v>144</v>
-      </c>
-      <c r="X22">
-        <v>138</v>
-      </c>
-      <c r="Y22">
-        <v>144</v>
-      </c>
-      <c r="Z22">
-        <v>136</v>
-      </c>
-      <c r="AA22">
-        <v>144</v>
-      </c>
-      <c r="AB22">
-        <v>138</v>
-      </c>
-      <c r="AC22">
-        <v>144</v>
-      </c>
-      <c r="AD22">
-        <v>144</v>
-      </c>
-      <c r="AE22">
-        <v>144</v>
-      </c>
-      <c r="AF22">
-        <v>144</v>
-      </c>
-      <c r="AG22">
-        <v>144</v>
-      </c>
-      <c r="AH22">
-        <f t="shared" si="4"/>
-        <v>144</v>
-      </c>
-      <c r="AI22">
-        <f t="shared" si="5"/>
-        <v>144</v>
-      </c>
-      <c r="AJ22">
-        <f t="shared" si="6"/>
-        <v>144</v>
-      </c>
-      <c r="AK22">
-        <f t="shared" si="7"/>
-        <v>144</v>
-      </c>
-      <c r="AL22">
-        <f t="shared" si="8"/>
-        <v>144</v>
-      </c>
-      <c r="AM22">
-        <f t="shared" si="9"/>
-        <v>144</v>
-      </c>
-      <c r="AN22">
-        <f t="shared" si="10"/>
-        <v>144</v>
-      </c>
-      <c r="AO22">
-        <f t="shared" si="11"/>
-        <v>144</v>
-      </c>
-      <c r="AP22">
-        <f t="shared" si="12"/>
-        <v>144</v>
-      </c>
-      <c r="AQ22">
-        <f t="shared" si="13"/>
-        <v>144</v>
-      </c>
-      <c r="AR22">
-        <f t="shared" si="14"/>
-        <v>144</v>
-      </c>
-      <c r="AS22">
-        <f t="shared" si="15"/>
-        <v>144</v>
-      </c>
-      <c r="AT22">
-        <f t="shared" si="16"/>
-        <v>144</v>
-      </c>
-      <c r="AU22">
-        <f t="shared" si="17"/>
-        <v>144</v>
-      </c>
-      <c r="AV22">
-        <f t="shared" si="18"/>
-        <v>144</v>
-      </c>
-      <c r="AW22">
-        <f t="shared" si="19"/>
-        <v>144</v>
-      </c>
-      <c r="AX22">
-        <f t="shared" si="20"/>
-        <v>144</v>
-      </c>
-      <c r="AY22">
-        <f t="shared" si="21"/>
-        <v>144</v>
-      </c>
-      <c r="AZ22">
-        <f t="shared" si="22"/>
-        <v>144</v>
-      </c>
-      <c r="BA22">
-        <f t="shared" si="23"/>
-        <v>144</v>
-      </c>
-      <c r="BB22">
-        <f t="shared" si="24"/>
-        <v>144</v>
-      </c>
-      <c r="BC22">
-        <f t="shared" si="25"/>
-        <v>144</v>
-      </c>
-      <c r="BD22">
-        <f t="shared" si="26"/>
-        <v>144</v>
-      </c>
-      <c r="BE22">
-        <f t="shared" si="27"/>
-        <v>144</v>
-      </c>
-      <c r="BF22">
-        <f t="shared" si="28"/>
-        <v>144</v>
-      </c>
-      <c r="BG22">
-        <f t="shared" si="29"/>
-        <v>144</v>
-      </c>
-      <c r="BH22">
-        <f t="shared" si="30"/>
-        <v>144</v>
-      </c>
-      <c r="BI22">
-        <f t="shared" si="31"/>
-        <v>144</v>
-      </c>
-      <c r="BJ22">
-        <f t="shared" si="32"/>
-        <v>144</v>
-      </c>
-      <c r="BK22">
-        <f t="shared" si="33"/>
-        <v>144</v>
-      </c>
-      <c r="BL22">
-        <f t="shared" si="34"/>
-        <v>144</v>
-      </c>
-      <c r="BM22">
-        <f t="shared" si="35"/>
-        <v>144</v>
-      </c>
-      <c r="BN22">
-        <f t="shared" si="36"/>
-        <v>144</v>
-      </c>
-      <c r="BO22">
-        <f t="shared" si="37"/>
-        <v>144</v>
-      </c>
-      <c r="BP22">
-        <f t="shared" si="38"/>
-        <v>144</v>
-      </c>
-      <c r="BQ22">
-        <f t="shared" si="39"/>
-        <v>144</v>
-      </c>
-      <c r="BR22">
-        <f t="shared" si="40"/>
-        <v>144</v>
-      </c>
-      <c r="BS22">
-        <f t="shared" si="41"/>
-        <v>144</v>
-      </c>
-      <c r="BT22">
-        <f t="shared" si="42"/>
-        <v>144</v>
-      </c>
-      <c r="BU22">
-        <f t="shared" si="43"/>
-        <v>144</v>
-      </c>
-      <c r="BV22">
-        <f t="shared" si="44"/>
-        <v>144</v>
-      </c>
-      <c r="BW22">
-        <f t="shared" si="45"/>
-        <v>144</v>
-      </c>
-      <c r="BX22">
-        <f t="shared" si="46"/>
-        <v>144</v>
-      </c>
-      <c r="BY22">
-        <f t="shared" si="47"/>
-        <v>144</v>
-      </c>
-      <c r="BZ22">
-        <f t="shared" si="48"/>
-        <v>144</v>
-      </c>
-      <c r="CA22">
-        <f t="shared" si="49"/>
-        <v>144</v>
-      </c>
-      <c r="CB22">
-        <f t="shared" si="50"/>
-        <v>144</v>
-      </c>
-      <c r="CC22">
-        <f t="shared" si="51"/>
-        <v>144</v>
-      </c>
-      <c r="CD22">
-        <f t="shared" si="52"/>
-        <v>144</v>
-      </c>
-      <c r="CE22">
-        <f t="shared" si="53"/>
-        <v>144</v>
-      </c>
-      <c r="CF22">
-        <f t="shared" si="54"/>
-        <v>144</v>
-      </c>
-      <c r="CG22">
-        <f t="shared" si="55"/>
-        <v>144</v>
-      </c>
-      <c r="CH22">
-        <f t="shared" si="56"/>
-        <v>144</v>
-      </c>
-      <c r="CI22">
-        <f t="shared" si="57"/>
-        <v>144</v>
-      </c>
-      <c r="CJ22">
-        <f t="shared" si="58"/>
-        <v>144</v>
-      </c>
-      <c r="CK22">
-        <f t="shared" si="59"/>
-        <v>144</v>
-      </c>
-      <c r="CL22">
-        <f t="shared" si="60"/>
-        <v>144</v>
-      </c>
-      <c r="CM22">
-        <f t="shared" si="61"/>
-        <v>144</v>
-      </c>
-      <c r="CN22">
-        <f t="shared" si="62"/>
-        <v>144</v>
-      </c>
-      <c r="CO22">
-        <f t="shared" si="63"/>
-        <v>144</v>
-      </c>
-      <c r="CP22">
-        <f t="shared" si="64"/>
-        <v>144</v>
-      </c>
-      <c r="CQ22">
-        <f t="shared" si="65"/>
-        <v>144</v>
-      </c>
-      <c r="CR22">
-        <f t="shared" si="66"/>
-        <v>144</v>
-      </c>
-      <c r="CS22">
-        <f t="shared" si="67"/>
-        <v>144</v>
-      </c>
-      <c r="CT22">
-        <f t="shared" si="68"/>
-        <v>144</v>
-      </c>
-      <c r="CU22">
-        <f t="shared" si="69"/>
-        <v>144</v>
-      </c>
-      <c r="CV22">
-        <f t="shared" si="70"/>
-        <v>144</v>
-      </c>
-      <c r="CW22">
-        <f t="shared" si="71"/>
-        <v>144</v>
-      </c>
-      <c r="CX22">
-        <f t="shared" si="72"/>
-        <v>144</v>
-      </c>
-      <c r="CY22">
-        <f t="shared" si="73"/>
-        <v>144</v>
-      </c>
-      <c r="CZ22">
-        <f t="shared" si="74"/>
-        <v>144</v>
-      </c>
-      <c r="DA22">
-        <f t="shared" si="75"/>
-        <v>144</v>
-      </c>
-      <c r="DB22">
-        <f t="shared" si="76"/>
-        <v>144</v>
-      </c>
-      <c r="DC22">
-        <f t="shared" si="77"/>
-        <v>144</v>
-      </c>
-      <c r="DD22">
-        <f t="shared" si="78"/>
-        <v>144</v>
-      </c>
-      <c r="DE22">
-        <f t="shared" si="79"/>
-        <v>144</v>
-      </c>
-      <c r="DF22">
-        <f t="shared" si="80"/>
-        <v>144</v>
-      </c>
-      <c r="DG22">
-        <f t="shared" si="81"/>
-        <v>144</v>
-      </c>
-      <c r="DH22">
-        <f t="shared" si="82"/>
-        <v>144</v>
-      </c>
-      <c r="DI22">
-        <f t="shared" si="83"/>
-        <v>144</v>
-      </c>
-      <c r="DJ22">
-        <f t="shared" si="84"/>
-        <v>144</v>
-      </c>
-      <c r="DK22">
-        <f t="shared" si="85"/>
-        <v>144</v>
-      </c>
-      <c r="DL22">
-        <f t="shared" si="86"/>
-        <v>144</v>
-      </c>
-      <c r="DM22">
-        <f t="shared" si="87"/>
-        <v>144</v>
-      </c>
-      <c r="DN22">
-        <f t="shared" si="88"/>
-        <v>144</v>
-      </c>
-      <c r="DO22">
-        <f t="shared" si="89"/>
-        <v>144</v>
-      </c>
-      <c r="DP22">
-        <f t="shared" si="90"/>
-        <v>144</v>
-      </c>
-      <c r="DQ22">
-        <f t="shared" si="91"/>
-        <v>144</v>
-      </c>
-      <c r="DR22">
-        <f t="shared" si="92"/>
-        <v>144</v>
-      </c>
-      <c r="DS22">
-        <f t="shared" si="93"/>
-        <v>144</v>
-      </c>
-      <c r="DT22">
-        <f t="shared" si="94"/>
-        <v>144</v>
-      </c>
-      <c r="DU22">
-        <f t="shared" si="95"/>
-        <v>144</v>
-      </c>
-      <c r="DV22">
-        <f t="shared" si="96"/>
-        <v>144</v>
-      </c>
-      <c r="DW22">
-        <f t="shared" si="97"/>
-        <v>144</v>
-      </c>
-      <c r="DX22">
-        <f t="shared" si="98"/>
-        <v>144</v>
-      </c>
-      <c r="DY22">
-        <f t="shared" si="99"/>
-        <v>144</v>
-      </c>
-      <c r="DZ22">
-        <f t="shared" si="100"/>
-        <v>144</v>
-      </c>
-      <c r="EA22">
-        <f t="shared" si="101"/>
-        <v>144</v>
-      </c>
-      <c r="EB22">
-        <f t="shared" si="102"/>
-        <v>144</v>
-      </c>
-      <c r="EC22">
-        <f t="shared" si="103"/>
-        <v>144</v>
-      </c>
-      <c r="ED22">
-        <f t="shared" si="104"/>
-        <v>144</v>
-      </c>
-      <c r="EE22">
-        <f t="shared" si="105"/>
-        <v>144</v>
-      </c>
-      <c r="EF22">
-        <f t="shared" si="106"/>
-        <v>144</v>
-      </c>
-      <c r="EG22">
-        <f t="shared" si="107"/>
-        <v>144</v>
-      </c>
     </row>
     <row r="23" spans="1:139" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
@@ -4315,517 +1478,6 @@
       </c>
       <c r="D23">
         <v>290</v>
-      </c>
-      <c r="F23">
-        <f>$C23</f>
-        <v>70</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="H23">
-        <f t="shared" ref="H23" si="128">G23</f>
-        <v>70</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="Q23">
-        <v>78</v>
-      </c>
-      <c r="R23">
-        <v>74</v>
-      </c>
-      <c r="S23">
-        <v>78</v>
-      </c>
-      <c r="T23">
-        <v>78</v>
-      </c>
-      <c r="U23">
-        <v>53</v>
-      </c>
-      <c r="V23">
-        <v>73</v>
-      </c>
-      <c r="W23">
-        <v>78</v>
-      </c>
-      <c r="X23">
-        <v>72</v>
-      </c>
-      <c r="Y23">
-        <v>78</v>
-      </c>
-      <c r="Z23">
-        <v>78</v>
-      </c>
-      <c r="AA23">
-        <v>78</v>
-      </c>
-      <c r="AB23">
-        <v>72</v>
-      </c>
-      <c r="AC23">
-        <v>78</v>
-      </c>
-      <c r="AD23">
-        <v>78</v>
-      </c>
-      <c r="AE23">
-        <v>78</v>
-      </c>
-      <c r="AF23">
-        <v>78</v>
-      </c>
-      <c r="AG23">
-        <v>78</v>
-      </c>
-      <c r="AH23">
-        <f t="shared" si="4"/>
-        <v>78</v>
-      </c>
-      <c r="AI23">
-        <f t="shared" si="5"/>
-        <v>78</v>
-      </c>
-      <c r="AJ23">
-        <f t="shared" si="6"/>
-        <v>78</v>
-      </c>
-      <c r="AK23">
-        <f t="shared" si="7"/>
-        <v>78</v>
-      </c>
-      <c r="AL23">
-        <f t="shared" si="8"/>
-        <v>78</v>
-      </c>
-      <c r="AM23">
-        <f t="shared" si="9"/>
-        <v>78</v>
-      </c>
-      <c r="AN23">
-        <f t="shared" si="10"/>
-        <v>78</v>
-      </c>
-      <c r="AO23">
-        <f t="shared" si="11"/>
-        <v>78</v>
-      </c>
-      <c r="AP23">
-        <f t="shared" si="12"/>
-        <v>78</v>
-      </c>
-      <c r="AQ23">
-        <f t="shared" si="13"/>
-        <v>78</v>
-      </c>
-      <c r="AR23">
-        <f t="shared" si="14"/>
-        <v>78</v>
-      </c>
-      <c r="AS23">
-        <f t="shared" si="15"/>
-        <v>78</v>
-      </c>
-      <c r="AT23">
-        <f t="shared" si="16"/>
-        <v>78</v>
-      </c>
-      <c r="AU23">
-        <f t="shared" si="17"/>
-        <v>78</v>
-      </c>
-      <c r="AV23">
-        <f t="shared" si="18"/>
-        <v>78</v>
-      </c>
-      <c r="AW23">
-        <f t="shared" si="19"/>
-        <v>78</v>
-      </c>
-      <c r="AX23">
-        <f t="shared" si="20"/>
-        <v>78</v>
-      </c>
-      <c r="AY23">
-        <f t="shared" si="21"/>
-        <v>78</v>
-      </c>
-      <c r="AZ23">
-        <f t="shared" si="22"/>
-        <v>78</v>
-      </c>
-      <c r="BA23">
-        <f t="shared" si="23"/>
-        <v>78</v>
-      </c>
-      <c r="BB23">
-        <f t="shared" si="24"/>
-        <v>78</v>
-      </c>
-      <c r="BC23">
-        <f t="shared" si="25"/>
-        <v>78</v>
-      </c>
-      <c r="BD23">
-        <f t="shared" si="26"/>
-        <v>78</v>
-      </c>
-      <c r="BE23">
-        <f t="shared" si="27"/>
-        <v>78</v>
-      </c>
-      <c r="BF23">
-        <f t="shared" si="28"/>
-        <v>78</v>
-      </c>
-      <c r="BG23">
-        <f t="shared" si="29"/>
-        <v>78</v>
-      </c>
-      <c r="BH23">
-        <f t="shared" si="30"/>
-        <v>78</v>
-      </c>
-      <c r="BI23">
-        <f t="shared" si="31"/>
-        <v>78</v>
-      </c>
-      <c r="BJ23">
-        <f t="shared" si="32"/>
-        <v>78</v>
-      </c>
-      <c r="BK23">
-        <f t="shared" si="33"/>
-        <v>78</v>
-      </c>
-      <c r="BL23">
-        <f t="shared" si="34"/>
-        <v>78</v>
-      </c>
-      <c r="BM23">
-        <f t="shared" si="35"/>
-        <v>78</v>
-      </c>
-      <c r="BN23">
-        <f t="shared" si="36"/>
-        <v>78</v>
-      </c>
-      <c r="BO23">
-        <f t="shared" si="37"/>
-        <v>78</v>
-      </c>
-      <c r="BP23">
-        <f t="shared" si="38"/>
-        <v>78</v>
-      </c>
-      <c r="BQ23">
-        <f t="shared" si="39"/>
-        <v>78</v>
-      </c>
-      <c r="BR23">
-        <f t="shared" si="40"/>
-        <v>78</v>
-      </c>
-      <c r="BS23">
-        <f t="shared" si="41"/>
-        <v>78</v>
-      </c>
-      <c r="BT23">
-        <f t="shared" si="42"/>
-        <v>78</v>
-      </c>
-      <c r="BU23">
-        <f t="shared" si="43"/>
-        <v>78</v>
-      </c>
-      <c r="BV23">
-        <f t="shared" si="44"/>
-        <v>78</v>
-      </c>
-      <c r="BW23">
-        <f t="shared" si="45"/>
-        <v>78</v>
-      </c>
-      <c r="BX23">
-        <f t="shared" si="46"/>
-        <v>78</v>
-      </c>
-      <c r="BY23">
-        <f t="shared" si="47"/>
-        <v>78</v>
-      </c>
-      <c r="BZ23">
-        <f t="shared" si="48"/>
-        <v>78</v>
-      </c>
-      <c r="CA23">
-        <f t="shared" si="49"/>
-        <v>78</v>
-      </c>
-      <c r="CB23">
-        <f t="shared" si="50"/>
-        <v>78</v>
-      </c>
-      <c r="CC23">
-        <f t="shared" si="51"/>
-        <v>78</v>
-      </c>
-      <c r="CD23">
-        <f t="shared" si="52"/>
-        <v>78</v>
-      </c>
-      <c r="CE23">
-        <f t="shared" si="53"/>
-        <v>78</v>
-      </c>
-      <c r="CF23">
-        <f t="shared" si="54"/>
-        <v>78</v>
-      </c>
-      <c r="CG23">
-        <f t="shared" si="55"/>
-        <v>78</v>
-      </c>
-      <c r="CH23">
-        <f t="shared" si="56"/>
-        <v>78</v>
-      </c>
-      <c r="CI23">
-        <f t="shared" si="57"/>
-        <v>78</v>
-      </c>
-      <c r="CJ23">
-        <f t="shared" si="58"/>
-        <v>78</v>
-      </c>
-      <c r="CK23">
-        <f t="shared" si="59"/>
-        <v>78</v>
-      </c>
-      <c r="CL23">
-        <f t="shared" si="60"/>
-        <v>78</v>
-      </c>
-      <c r="CM23">
-        <f t="shared" si="61"/>
-        <v>78</v>
-      </c>
-      <c r="CN23">
-        <f t="shared" si="62"/>
-        <v>78</v>
-      </c>
-      <c r="CO23">
-        <f t="shared" si="63"/>
-        <v>78</v>
-      </c>
-      <c r="CP23">
-        <f t="shared" si="64"/>
-        <v>78</v>
-      </c>
-      <c r="CQ23">
-        <f t="shared" si="65"/>
-        <v>78</v>
-      </c>
-      <c r="CR23">
-        <f t="shared" si="66"/>
-        <v>78</v>
-      </c>
-      <c r="CS23">
-        <f t="shared" si="67"/>
-        <v>78</v>
-      </c>
-      <c r="CT23">
-        <f t="shared" si="68"/>
-        <v>78</v>
-      </c>
-      <c r="CU23">
-        <f t="shared" si="69"/>
-        <v>78</v>
-      </c>
-      <c r="CV23">
-        <f t="shared" si="70"/>
-        <v>78</v>
-      </c>
-      <c r="CW23">
-        <f t="shared" si="71"/>
-        <v>78</v>
-      </c>
-      <c r="CX23">
-        <f t="shared" si="72"/>
-        <v>78</v>
-      </c>
-      <c r="CY23">
-        <f t="shared" si="73"/>
-        <v>78</v>
-      </c>
-      <c r="CZ23">
-        <f t="shared" si="74"/>
-        <v>78</v>
-      </c>
-      <c r="DA23">
-        <f t="shared" si="75"/>
-        <v>78</v>
-      </c>
-      <c r="DB23">
-        <f t="shared" si="76"/>
-        <v>78</v>
-      </c>
-      <c r="DC23">
-        <f t="shared" si="77"/>
-        <v>78</v>
-      </c>
-      <c r="DD23">
-        <f t="shared" si="78"/>
-        <v>78</v>
-      </c>
-      <c r="DE23">
-        <f t="shared" si="79"/>
-        <v>78</v>
-      </c>
-      <c r="DF23">
-        <f t="shared" si="80"/>
-        <v>78</v>
-      </c>
-      <c r="DG23">
-        <f t="shared" si="81"/>
-        <v>78</v>
-      </c>
-      <c r="DH23">
-        <f t="shared" si="82"/>
-        <v>78</v>
-      </c>
-      <c r="DI23">
-        <f t="shared" si="83"/>
-        <v>78</v>
-      </c>
-      <c r="DJ23">
-        <f t="shared" si="84"/>
-        <v>78</v>
-      </c>
-      <c r="DK23">
-        <f t="shared" si="85"/>
-        <v>78</v>
-      </c>
-      <c r="DL23">
-        <f t="shared" si="86"/>
-        <v>78</v>
-      </c>
-      <c r="DM23">
-        <f t="shared" si="87"/>
-        <v>78</v>
-      </c>
-      <c r="DN23">
-        <f t="shared" si="88"/>
-        <v>78</v>
-      </c>
-      <c r="DO23">
-        <f t="shared" si="89"/>
-        <v>78</v>
-      </c>
-      <c r="DP23">
-        <f t="shared" si="90"/>
-        <v>78</v>
-      </c>
-      <c r="DQ23">
-        <f t="shared" si="91"/>
-        <v>78</v>
-      </c>
-      <c r="DR23">
-        <f t="shared" si="92"/>
-        <v>78</v>
-      </c>
-      <c r="DS23">
-        <f t="shared" si="93"/>
-        <v>78</v>
-      </c>
-      <c r="DT23">
-        <f t="shared" si="94"/>
-        <v>78</v>
-      </c>
-      <c r="DU23">
-        <f t="shared" si="95"/>
-        <v>78</v>
-      </c>
-      <c r="DV23">
-        <f t="shared" si="96"/>
-        <v>78</v>
-      </c>
-      <c r="DW23">
-        <f t="shared" si="97"/>
-        <v>78</v>
-      </c>
-      <c r="DX23">
-        <f t="shared" si="98"/>
-        <v>78</v>
-      </c>
-      <c r="DY23">
-        <f t="shared" si="99"/>
-        <v>78</v>
-      </c>
-      <c r="DZ23">
-        <f t="shared" si="100"/>
-        <v>78</v>
-      </c>
-      <c r="EA23">
-        <f t="shared" si="101"/>
-        <v>78</v>
-      </c>
-      <c r="EB23">
-        <f t="shared" si="102"/>
-        <v>78</v>
-      </c>
-      <c r="EC23">
-        <f t="shared" si="103"/>
-        <v>78</v>
-      </c>
-      <c r="ED23">
-        <f t="shared" si="104"/>
-        <v>78</v>
-      </c>
-      <c r="EE23">
-        <f t="shared" si="105"/>
-        <v>78</v>
-      </c>
-      <c r="EF23">
-        <f t="shared" si="106"/>
-        <v>78</v>
-      </c>
-      <c r="EG23">
-        <f t="shared" si="107"/>
-        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:139" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Projekte löschen (in DB) mit frmDeleteProjects zum Auswählen der zu löschenden TimeStamps. Alle DB-Sätze die gelöscht werden, werden in die 'databaseName'Trash-DB gesichert. Korrigieren des variantName: nun überall "" und nicht Nothing neue DatenbankProzedur: deleteProjectsinDB
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/bin/Debug/requirements/Project Board Customization.xlsx
+++ b/Projectboard/Projectboard/bin/Debug/requirements/Project Board Customization.xlsx
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="138">
   <si>
     <t xml:space="preserve">Customization - Einstellung der Parameter </t>
   </si>
@@ -521,6 +521,9 @@
   </si>
   <si>
     <t>special Phase (LeLe)</t>
+  </si>
+  <si>
+    <t>ITProjekte2</t>
   </si>
 </sst>
 </file>
@@ -1168,8 +1171,8 @@
   <dimension ref="A1:EI68"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="EH22" sqref="EH22"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1720,7 +1723,7 @@
         <v>86</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
Einchecken Project Board customization mit Feld "Zeitraum Farbe festlegen"
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/bin/Debug/requirements/Project Board Customization.xlsx
+++ b/Projectboard/Projectboard/bin/Debug/requirements/Project Board Customization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr updateLinks="always" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showSheetTabs="0" xWindow="120" yWindow="192" windowWidth="15600" windowHeight="11640"/>
+    <workbookView showSheetTabs="0" xWindow="120" yWindow="195" windowWidth="15600" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Einstellungen" sheetId="4" r:id="rId1"/>
@@ -25,20 +25,21 @@
     <definedName name="awin_Phasen_Definition">Einstellungen!$B$7:$B$14</definedName>
     <definedName name="awin_Projekt_Definition">Einstellungen!#REF!</definedName>
     <definedName name="awin_Rollen_Definition">Einstellungen!$B$17:$B$24</definedName>
-    <definedName name="_xlnm.Database">Einstellungen!$B$64</definedName>
-    <definedName name="EinzelRessourcenExport">Einstellungen!$B$68</definedName>
+    <definedName name="_xlnm.Database">Einstellungen!$B$65</definedName>
+    <definedName name="EinzelRessourcenExport">Einstellungen!$B$69</definedName>
     <definedName name="Ergebnisfarbe1">Einstellungen!$B$49</definedName>
     <definedName name="Ergebnisfarbe2">Einstellungen!$B$50</definedName>
     <definedName name="Farbe_externe_Ressourcen">Einstellungen!$B$43</definedName>
     <definedName name="Farbe_für_Projekte_ohne_Vorlage">Einstellungen!$B$44</definedName>
     <definedName name="Farbe_intern_ohne_Projekte">Einstellungen!$B$42</definedName>
     <definedName name="Farbe_Ress_Kost_Werte">Einstellungen!$B$45</definedName>
+    <definedName name="FarbeZeitraum">Einstellungen!$B$59</definedName>
     <definedName name="GlowColor">Einstellungen!$B$58</definedName>
-    <definedName name="kapaEinheit">Einstellungen!$B$62</definedName>
+    <definedName name="kapaEinheit">Einstellungen!$B$63</definedName>
     <definedName name="Linker_Rand_Ressourcen_Diagramme">Einstellungen!$B$37</definedName>
     <definedName name="Max_Dauer_eines_Projektes">Einstellungen!$B$36</definedName>
     <definedName name="NoShow_Time_Zone_Color">Einstellungen!$B$40</definedName>
-    <definedName name="offsetEinheit">Einstellungen!$B$63</definedName>
+    <definedName name="offsetEinheit">Einstellungen!$B$64</definedName>
     <definedName name="P1_CostDefinition">'Projektdefinition Kosten'!$A$2:$A$18</definedName>
     <definedName name="P1_Definition">'Projektdefinition Ressourcen'!$A$2:$A$19</definedName>
     <definedName name="P2_CostDefinition">'Projektdefinition Kosten'!$A$21:$A$31</definedName>
@@ -61,15 +62,15 @@
     <definedName name="Soll_Ist_Farbe_Aktuell">Einstellungen!$B$53</definedName>
     <definedName name="Soll_Ist_Farbe_Beauftragung">Einstellungen!$B$51</definedName>
     <definedName name="Soll_Ist_Farbe_letzte_Freigabe">Einstellungen!$B$52</definedName>
-    <definedName name="Spaltenbreite">Einstellungen!$B$67</definedName>
-    <definedName name="Start_Kalender">Einstellungen!$B$60</definedName>
+    <definedName name="Spaltenbreite">Einstellungen!$B$68</definedName>
+    <definedName name="Start_Kalender">Einstellungen!$B$61</definedName>
     <definedName name="Vergleichsfarbe1">Einstellungen!$B$46</definedName>
     <definedName name="Vergleichsfarbe2">Einstellungen!$B$47</definedName>
     <definedName name="Vergleichsfarbe3">Einstellungen!$B$48</definedName>
-    <definedName name="WeightStrategicFit">Einstellungen!$B$59</definedName>
-    <definedName name="Zeilenhoehe1">Einstellungen!$B$65</definedName>
-    <definedName name="Zeilenhoehe2">Einstellungen!$B$66</definedName>
-    <definedName name="Zeiteinheit">Einstellungen!$B$61</definedName>
+    <definedName name="WeightStrategicFit">Einstellungen!$B$60</definedName>
+    <definedName name="Zeilenhoehe1">Einstellungen!$B$66</definedName>
+    <definedName name="Zeilenhoehe2">Einstellungen!$B$67</definedName>
+    <definedName name="Zeiteinheit">Einstellungen!$B$62</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -81,7 +82,7 @@
     <author>tom</author>
   </authors>
   <commentList>
-    <comment ref="L64" authorId="0">
+    <comment ref="L65" authorId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="139">
   <si>
     <t xml:space="preserve">Customization - Einstellung der Parameter </t>
   </si>
@@ -523,7 +524,10 @@
     <t>special Phase (LeLe)</t>
   </si>
   <si>
-    <t>ITProjekte2</t>
+    <t>Farbe zur Markierung Zeitraum in der Projekttafel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wenn 1: dann wird die TimeSpan mit der angegebenen Farbe angezeigt ; wenn 0, dann nicht </t>
   </si>
 </sst>
 </file>
@@ -1168,20 +1172,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:EI68"/>
+  <dimension ref="A1:EI69"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="22" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59:D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+    <col min="1" max="1" width="47.7109375" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="30.109375" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
@@ -1189,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -1197,22 +1201,22 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="41" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="40" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -1223,7 +1227,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="37" t="s">
         <v>117</v>
       </c>
@@ -1234,42 +1238,42 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" s="28" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" s="38" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="34" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:139" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1417,7 +1421,7 @@
       <c r="EH17" s="30"/>
       <c r="EI17" s="30"/>
     </row>
-    <row r="18" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="35" t="s">
         <v>12</v>
       </c>
@@ -1428,7 +1432,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="19" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="20" t="s">
         <v>126</v>
       </c>
@@ -1439,7 +1443,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="28" t="s">
         <v>118</v>
       </c>
@@ -1450,7 +1454,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="21" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B21" s="27" t="s">
         <v>127</v>
       </c>
@@ -1461,7 +1465,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="22" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" s="29" t="s">
         <v>119</v>
       </c>
@@ -1472,7 +1476,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="23" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>120</v>
       </c>
@@ -1483,53 +1487,53 @@
         <v>290</v>
       </c>
     </row>
-    <row r="24" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:139" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="42" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:139" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B30" s="36"/>
     </row>
-    <row r="31" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:139" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:139" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1537,7 +1541,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1545,7 +1549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1553,19 +1557,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>25</v>
       </c>
       <c r="B39" s="10"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="11"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>27</v>
       </c>
@@ -1573,215 +1577,226 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>28</v>
       </c>
       <c r="B42" s="21"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>29</v>
       </c>
       <c r="B43" s="12"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>30</v>
       </c>
       <c r="B44" s="13"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>31</v>
       </c>
       <c r="B45" s="14"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>78</v>
       </c>
       <c r="B46" s="10"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>79</v>
       </c>
       <c r="B47" s="9"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>80</v>
       </c>
       <c r="B48" s="19"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>81</v>
       </c>
       <c r="B49" s="20"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>82</v>
       </c>
       <c r="B50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>94</v>
       </c>
       <c r="B51" s="25"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>95</v>
       </c>
       <c r="B52" s="24"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>96</v>
       </c>
       <c r="B53" s="26"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>100</v>
       </c>
       <c r="B54" s="34"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>97</v>
       </c>
       <c r="B55" s="35"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>98</v>
       </c>
       <c r="B56" s="36"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>99</v>
       </c>
       <c r="B57" s="11"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>101</v>
       </c>
       <c r="B58" s="36"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>137</v>
+      </c>
+      <c r="B59" s="14">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>83</v>
       </c>
-      <c r="B59">
+      <c r="B60">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="61" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="18">
+      <c r="B61" s="18">
         <v>41153</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="62" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B62" s="22" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>110</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B63" s="22" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>131</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B64" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="65" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>86</v>
       </c>
-      <c r="B64" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="D64" s="22" t="s">
+      <c r="B65" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="E64" s="22" t="s">
+      <c r="E65" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>106</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G65" t="s">
         <v>107</v>
       </c>
-      <c r="H64" s="22" t="s">
+      <c r="H65" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="I64" s="22" t="s">
+      <c r="I65" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="J64" s="22" t="s">
+      <c r="J65" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="K64" s="22" t="s">
+      <c r="K65" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="L64" s="22" t="s">
+      <c r="L65" s="22" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="66" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>90</v>
       </c>
-      <c r="B65" s="23">
+      <c r="B66" s="23">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="67" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>91</v>
       </c>
-      <c r="B66" s="23">
+      <c r="B67" s="23">
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="68" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>92</v>
       </c>
-      <c r="B67" s="23">
+      <c r="B68" s="23">
         <v>3.4</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="69" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>109</v>
       </c>
-      <c r="B68" s="32">
+      <c r="B69" s="32">
         <v>1</v>
       </c>
     </row>
@@ -1803,13 +1818,13 @@
       <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="63" width="4.33203125" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="63" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>32</v>
       </c>
@@ -1997,7 +2012,7 @@
       <c r="BK1" s="15"/>
       <c r="BL1" s="15"/>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2023,7 +2038,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
@@ -2079,7 +2094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
         <v>13</v>
       </c>
@@ -2135,7 +2150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
@@ -2192,7 +2207,7 @@
       <c r="Y6" s="16"/>
       <c r="Z6" s="16"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" s="16" t="s">
         <v>14</v>
       </c>
@@ -2225,7 +2240,7 @@
       <c r="Y7" s="16"/>
       <c r="Z7" s="16"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
@@ -2282,7 +2297,7 @@
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="16" t="s">
         <v>14</v>
@@ -2322,7 +2337,7 @@
       <c r="Y10" s="16"/>
       <c r="Z10" s="16"/>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -2380,7 +2395,7 @@
       <c r="Y12" s="16"/>
       <c r="Z12" s="16"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="16" t="s">
         <v>14</v>
@@ -2416,7 +2431,7 @@
       <c r="Y13" s="16"/>
       <c r="Z13" s="16"/>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="16" t="s">
         <v>15</v>
@@ -2452,7 +2467,7 @@
       <c r="Y14" s="16"/>
       <c r="Z14" s="16"/>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -2510,7 +2525,7 @@
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="16" t="s">
         <v>14</v>
@@ -2554,7 +2569,7 @@
       <c r="Y17" s="16"/>
       <c r="Z17" s="16"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="16" t="s">
         <v>16</v>
@@ -2598,7 +2613,7 @@
       <c r="Y18" s="16"/>
       <c r="Z18" s="16"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -2626,7 +2641,7 @@
       <c r="Y19" s="16"/>
       <c r="Z19" s="16"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -2654,7 +2669,7 @@
       <c r="Y20" s="16"/>
       <c r="Z20" s="16"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -2682,7 +2697,7 @@
       <c r="Y21" s="16"/>
       <c r="Z21" s="16"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
@@ -2699,7 +2714,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="16" t="s">
         <v>12</v>
       </c>
@@ -2740,7 +2755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="16" t="s">
         <v>13</v>
       </c>
@@ -2781,7 +2796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
@@ -2806,7 +2821,7 @@
       <c r="R26" s="16"/>
       <c r="S26" s="16"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16" t="s">
         <v>14</v>
@@ -2835,7 +2850,7 @@
       <c r="R27" s="16"/>
       <c r="S27" s="16"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -2879,7 +2894,7 @@
       <c r="R29" s="16"/>
       <c r="S29" s="16"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="16" t="s">
         <v>14</v>
@@ -2908,7 +2923,7 @@
       <c r="R30" s="16"/>
       <c r="S30" s="16"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="16" t="s">
         <v>15</v>
@@ -2937,7 +2952,7 @@
       <c r="R31" s="16"/>
       <c r="S31" s="16"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -2981,7 +2996,7 @@
       <c r="R33" s="16"/>
       <c r="S33" s="16"/>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="16" t="s">
         <v>14</v>
@@ -3016,7 +3031,7 @@
       <c r="R34" s="16"/>
       <c r="S34" s="16"/>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="16" t="s">
         <v>16</v>
@@ -3051,7 +3066,7 @@
       <c r="R35" s="16"/>
       <c r="S35" s="16"/>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -3079,7 +3094,7 @@
       <c r="Y36" s="16"/>
       <c r="Z36" s="16"/>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -3107,7 +3122,7 @@
       <c r="Y37" s="16"/>
       <c r="Z37" s="16"/>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>4</v>
       </c>
@@ -3142,7 +3157,7 @@
       <c r="AE39" s="16"/>
       <c r="AF39" s="16"/>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B40" s="16" t="s">
         <v>12</v>
       </c>
@@ -3191,7 +3206,7 @@
       <c r="AE40" s="16"/>
       <c r="AF40" s="16"/>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B41" s="16" t="s">
         <v>13</v>
       </c>
@@ -3240,7 +3255,7 @@
       <c r="AE41" s="16"/>
       <c r="AF41" s="16"/>
     </row>
-    <row r="43" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>7</v>
       </c>
@@ -3258,7 +3273,7 @@
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="16" t="s">
         <v>14</v>
@@ -3292,7 +3307,7 @@
       <c r="Y44" s="16"/>
       <c r="Z44" s="16"/>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="16" t="s">
         <v>15</v>
@@ -3326,7 +3341,7 @@
       <c r="Y45" s="16"/>
       <c r="Z45" s="16"/>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -3354,7 +3369,7 @@
       <c r="Y46" s="16"/>
       <c r="Z46" s="16"/>
     </row>
-    <row r="47" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>8</v>
       </c>
@@ -3384,7 +3399,7 @@
       <c r="Y47" s="16"/>
       <c r="Z47" s="16"/>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
         <v>14</v>
       </c>
@@ -3423,7 +3438,7 @@
       <c r="Y48" s="16"/>
       <c r="Z48" s="16"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="16"/>
       <c r="B49" s="16" t="s">
         <v>16</v>
@@ -3463,7 +3478,7 @@
       <c r="Y49" s="16"/>
       <c r="Z49" s="16"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="16"/>
       <c r="C50" s="16"/>
       <c r="D50" s="16"/>
@@ -3472,7 +3487,7 @@
       <c r="G50" s="16"/>
       <c r="H50" s="16"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O51" s="16"/>
       <c r="P51" s="16"/>
       <c r="Q51" s="16"/>
@@ -3496,13 +3511,13 @@
       <selection activeCell="A34" sqref="A34:A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="62" width="4.33203125" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="62" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>32</v>
       </c>
@@ -3688,7 +3703,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3714,7 +3729,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>20</v>
       </c>
@@ -3770,7 +3785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -3797,7 +3812,7 @@
       <c r="Y4" s="16"/>
       <c r="Z4" s="16"/>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>33</v>
       </c>
@@ -3827,7 +3842,7 @@
       <c r="Y5" s="16"/>
       <c r="Z5" s="16"/>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B6" s="16" t="s">
         <v>20</v>
       </c>
@@ -3860,7 +3875,7 @@
       <c r="Y6" s="16"/>
       <c r="Z6" s="16"/>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -3887,7 +3902,7 @@
       <c r="Y7" s="16"/>
       <c r="Z7" s="16"/>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>34</v>
       </c>
@@ -3917,7 +3932,7 @@
       <c r="Y8" s="16"/>
       <c r="Z8" s="16"/>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="16" t="s">
         <v>19</v>
@@ -3957,7 +3972,7 @@
       <c r="Y9" s="16"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="16" t="s">
         <v>20</v>
@@ -3997,7 +4012,7 @@
       <c r="Y10" s="16"/>
       <c r="Z10" s="16"/>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -4025,7 +4040,7 @@
       <c r="Y11" s="16"/>
       <c r="Z11" s="16"/>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>35</v>
       </c>
@@ -4055,7 +4070,7 @@
       <c r="Y12" s="16"/>
       <c r="Z12" s="16"/>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="16" t="s">
         <v>19</v>
@@ -4091,7 +4106,7 @@
       <c r="Y13" s="16"/>
       <c r="Z13" s="16"/>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -4119,7 +4134,7 @@
       <c r="Y14" s="16"/>
       <c r="Z14" s="16"/>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>36</v>
       </c>
@@ -4149,7 +4164,7 @@
       <c r="Y15" s="16"/>
       <c r="Z15" s="16"/>
     </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:62" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="16" t="s">
         <v>18</v>
@@ -4193,7 +4208,7 @@
       <c r="Y16" s="16"/>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="16" t="s">
         <v>20</v>
@@ -4237,7 +4252,7 @@
       <c r="Y17" s="16"/>
       <c r="Z17" s="16"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -4265,7 +4280,7 @@
       <c r="Y18" s="16"/>
       <c r="Z18" s="16"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -4293,7 +4308,7 @@
       <c r="Y19" s="16"/>
       <c r="Z19" s="16"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -4321,7 +4336,7 @@
       <c r="Y20" s="16"/>
       <c r="Z20" s="16"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -4338,14 +4353,14 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>34</v>
       </c>
@@ -4355,7 +4370,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="16"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="16" t="s">
         <v>19</v>
@@ -4391,7 +4406,7 @@
       <c r="Y24" s="16"/>
       <c r="Z24" s="16"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -4419,7 +4434,7 @@
       <c r="Y25" s="16"/>
       <c r="Z25" s="16"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>35</v>
       </c>
@@ -4449,7 +4464,7 @@
       <c r="Y26" s="16"/>
       <c r="Z26" s="16"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16" t="s">
         <v>19</v>
@@ -4485,7 +4500,7 @@
       <c r="Y27" s="16"/>
       <c r="Z27" s="16"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -4513,7 +4528,7 @@
       <c r="Y28" s="16"/>
       <c r="Z28" s="16"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>36</v>
       </c>
@@ -4543,7 +4558,7 @@
       <c r="Y29" s="16"/>
       <c r="Z29" s="16"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="16" t="s">
         <v>18</v>
@@ -4585,7 +4600,7 @@
       <c r="Y30" s="16"/>
       <c r="Z30" s="16"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -4613,7 +4628,7 @@
       <c r="Y31" s="16"/>
       <c r="Z31" s="16"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -4641,7 +4656,7 @@
       <c r="Y32" s="16"/>
       <c r="Z32" s="16"/>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>4</v>
       </c>
@@ -4653,7 +4668,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B35" s="16" t="s">
         <v>20</v>
       </c>
@@ -4702,14 +4717,14 @@
       <c r="AE35" s="16"/>
       <c r="AF35" s="16"/>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B38" s="16" t="s">
         <v>19</v>
       </c>
@@ -4742,10 +4757,10 @@
       <c r="Y38" s="16"/>
       <c r="Z38" s="16"/>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B39" s="16"/>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>36</v>
       </c>
@@ -4756,7 +4771,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16" t="s">
         <v>18</v>
@@ -4789,7 +4804,7 @@
       <c r="R41" s="16"/>
       <c r="S41" s="16"/>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16" t="s">
         <v>20</v>
@@ -4838,19 +4853,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -4876,7 +4891,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -4902,7 +4917,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -4928,7 +4943,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4954,7 +4969,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -4980,7 +4995,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -5006,7 +5021,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -5032,7 +5047,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -5058,7 +5073,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -5084,7 +5099,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -5110,7 +5125,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -5136,7 +5151,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -5162,7 +5177,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -5188,7 +5203,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -5214,7 +5229,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -5240,7 +5255,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -5266,7 +5281,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -5292,7 +5307,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -5318,7 +5333,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -5344,7 +5359,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -5370,7 +5385,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -5396,7 +5411,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -5422,7 +5437,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -5448,7 +5463,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -5474,7 +5489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -5500,7 +5515,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -5526,7 +5541,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -5552,7 +5567,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -5578,7 +5593,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -5604,7 +5619,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -5630,7 +5645,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -5656,7 +5671,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>61</v>
       </c>

</xml_diff>